<commit_message>
🙈✨ Updating .gitignore file. Adding all content to test plan of Tienda Cereza
</commit_message>
<xml_diff>
--- a/PlanDePruebasRiesgosCasosDePrueba.xlsx
+++ b/PlanDePruebasRiesgosCasosDePrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\Training\Duras\Repos\C1-2023-QA-Calidad-T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219B87BD-6C83-4305-BF7A-CC3E838606C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DCCA6A-27A7-4526-A842-9F4322670DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="6" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
   </bookViews>
   <sheets>
     <sheet name="PlaneDePruebaServicios" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="104">
   <si>
     <t>Célula</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Célula 2</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Funcionamiento de los microservicios de la pagina reqres.in </t>
-  </si>
-  <si>
     <t xml:space="preserve">Área </t>
   </si>
   <si>
@@ -102,6 +99,387 @@
   </si>
   <si>
     <t>Estudiante de SofkaU</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Abarca la ejecución de las pruebas funcionales para la petición GET LIST USERS en el canal: https://reqres.in</t>
+  </si>
+  <si>
+    <t>Abarca la ejecución de las pruebas funcionales para la petición POST REGISTER en el canal: https://reqres.in</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">No hace parte del alcance:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No es objeto de prueba la verificación de funcionalidades que no hagan parte de la petición GET LIST USERS.
+Tampoco se tendrá en cuenta pruebas de seguridad, rendimiento y estrés.</t>
+    </r>
+  </si>
+  <si>
+    <t>Las actividades descritas en el alcance se realizarán en el transcurso del 27 de febrero en las horas 11:00 AM a 12:00 PM.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">No hace parte del alcance:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No es objeto de prueba la verificación de funcionalidades que no hagan parte de la petición POST REGISTER.
+Tampoco se tendrá en cuenta pruebas de seguridad, rendimiento y estrés.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Hace parte del alcance:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1. Verificar que un usuario NO definido NO se puede registrar.
+2. Verificar la visualización del mensaje de error cuando el campo de contraseña está vacío.
+3. Verificar la visualización del mensaje de error cuando el campo de correo está vacío.
+4. Verificar que la contraseña contenga mínimo 8 caracteres.</t>
+    </r>
+  </si>
+  <si>
+    <t>N°</t>
+  </si>
+  <si>
+    <t>Identificador</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Pre-Condición</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entradas </t>
+  </si>
+  <si>
+    <t>Pasos Caso Prueba</t>
+  </si>
+  <si>
+    <t>Resultado Esperado</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>CA01</t>
+  </si>
+  <si>
+    <t>Verificar si la respuesta al realizar la petición adecuadamente es la correcta (200 OK).</t>
+  </si>
+  <si>
+    <t>La pagina https://reqres.in debe estar en funcionamiento.</t>
+  </si>
+  <si>
+    <t>Estando dentro del entorno descrito en el apartado de contexto de la sección Alcance:
+1. Ingresar a la aplicación Postman.
+2. Crear una nueva HTTP Request de tipo GET.
+3. Ingresar la URL https://reqres.in/api/users?page=2 a esta petición.
+4. Enviarla.
+5. Revisar si la respuesta es la correcta.</t>
+  </si>
+  <si>
+    <t>Recibir una respuesta con el STATUS: 200 OK.</t>
+  </si>
+  <si>
+    <t>Pasó</t>
+  </si>
+  <si>
+    <t>Terminado</t>
+  </si>
+  <si>
+    <t>CA02</t>
+  </si>
+  <si>
+    <t>Verificar que el contenido de la respuesta corresponda al formato adecuado (JSON).</t>
+  </si>
+  <si>
+    <t>Estando dentro del entorno descrito en el apartado de contexto de la sección Alcance:
+1. Identificar los parámetros de la solicitud de la API.
+2. Ingresar a la aplicación Postman.
+3. Crear una nueva HTTP Request de tipo GET.
+4. Ingresar la URL https://reqres.in/api/users?page=2 a esta petición.
+5. Enviarla.
+6. Revisar que el cuerpo de la respuesta de la petición sea el correspondiente en el formato JSON.</t>
+  </si>
+  <si>
+    <t>Recibir una respuesta en formato JSON, así:
+{
+    "id": 1,
+    "email": "email@email.com",
+    "first_name": "nombre",
+    "last_name": "apellido",
+    "avatar": "imange.jpg"
+ }</t>
+  </si>
+  <si>
+    <t>CA03</t>
+  </si>
+  <si>
+    <t>Verificar que al enviar un valor adecuado al parámetro, la respuesta sea aceptada.</t>
+  </si>
+  <si>
+    <t>Estando dentro del entorno descrito en el apartado de contexto de la sección Alcance:
+1. Ingresar a la aplicación Postman.
+2. Crear una nueva HTTP Request de tipo GET.
+3. Ingresar la URL https://reqres.in/api/users?page=2 a esta petición.
+4. Enviarla.
+5. Revisar si la respuesta a la petición es la correcta.</t>
+  </si>
+  <si>
+    <t>Recibir respuesta a la petición con el body indicado.</t>
+  </si>
+  <si>
+    <t>CA04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificar que al enviar un valor inadecuado al parámetro, la respuesta sea fallida. </t>
+  </si>
+  <si>
+    <t>Estando dentro del entorno descrito en el apartado de contexto de la sección Alcance:
+1. Ingresar a la aplicación Postman.
+2. Crear una nueva HTTP Request de tipo GET.
+3. Ingresar la URL https://reqres.in/api/users?page=%!"@#;¨^.
+4. Enviarla.
+5. Revisar si la respuesta a la petición es fallida.</t>
+  </si>
+  <si>
+    <t>Recibir una respuesta fallida a la petición.</t>
+  </si>
+  <si>
+    <t>No pasó</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Impacto</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Probabilidad de ocurrencia</t>
+  </si>
+  <si>
+    <t>Severidad</t>
+  </si>
+  <si>
+    <t>Nivel de riesgo</t>
+  </si>
+  <si>
+    <t>Acción</t>
+  </si>
+  <si>
+    <t>Plan de Acción</t>
+  </si>
+  <si>
+    <t>Mala determinación del tipo de respuesta HTTP.</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>Ignorar</t>
+  </si>
+  <si>
+    <t>Revisión y validación de la respuesta HTTP antes de permitir recibir peticiones.</t>
+  </si>
+  <si>
+    <t>Estructura JSON con formato erróneo.</t>
+  </si>
+  <si>
+    <t>Mitigar</t>
+  </si>
+  <si>
+    <t>Reestructurar el JSON a ser entregado de la manera correcta.</t>
+  </si>
+  <si>
+    <t>La petición no es aceptada a pesar de enviar un valor de parámetro correcto.</t>
+  </si>
+  <si>
+    <t>Contener</t>
+  </si>
+  <si>
+    <t>Revisar el codigo detrás de la petición y cambiar la parte de validación del parametro recibido.</t>
+  </si>
+  <si>
+    <t>La petición es aceptada a pesar de enviar un valor de parámetro incorrecto.</t>
+  </si>
+  <si>
+    <t>Un usuario que está definido, no se puede registrar.</t>
+  </si>
+  <si>
+    <t>Realizar una correcta asociación entre la definición de usuario y el sistema de registro.</t>
+  </si>
+  <si>
+    <t>Se registra un usuario con contraseña vacía.</t>
+  </si>
+  <si>
+    <t>Realizar una correcta definición de las reglas para la aceptación de una contraseña como válida.</t>
+  </si>
+  <si>
+    <t>Se registra un usuario con correo vacío.</t>
+  </si>
+  <si>
+    <t>Realizar una correcta definición de las reglas para la aceptación de un correo como válido.</t>
+  </si>
+  <si>
+    <t>Se registra un usuario con contraseña de menos de 5 caracteres.</t>
+  </si>
+  <si>
+    <t>Transferir</t>
+  </si>
+  <si>
+    <t>Informar del defecto al equipo de desarrollo.</t>
+  </si>
+  <si>
+    <t>Se probará la respuesta de la petición.
+Se probará el URL de la petición realizando cambios en el parámetro de la página.</t>
+  </si>
+  <si>
+    <t>Abarca la ejecución de las pruebas funcionales para el registro de usuarios en el canal: https://tiendacereza.com/</t>
+  </si>
+  <si>
+    <t>Abarca la ejecución de las pruebas funcionales para el ingreso de usuarios en el canal: https://tiendacereza.com/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">No hace parte del alcance:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No es objeto de prueba la verificación de funcionalidades que no hagan parte del sistema de ingreso en la Tienda Cereza 🍒.
+Tampoco se tendrá en cuenta pruebas de seguridad, rendimiento y estrés.</t>
+    </r>
+  </si>
+  <si>
+    <t>Las actividades descritas en el alcance se realizarán en el transcurso del 27 de febrero en las horas 12:00 PM a 01:00 PM.</t>
+  </si>
+  <si>
+    <t>Las actividades descritas en el alcance se realizarán en el transcurso del 27 de febrero en las horas 02:30 PM a 03:30 PM.</t>
+  </si>
+  <si>
+    <t>Las actividades descritas en el alcance se realizarán en el transcurso del 27 de febrero en las horas 03:30 PM a 04:25 PM.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">No hace parte del alcance:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No es objeto de prueba la verificación de funcionalidades que no hagan parte del sistema de resgistro en la Tienda Cereza 🍒.
+Tampoco se tendrá en cuenta pruebas de seguridad, rendimiento y estrés.</t>
+    </r>
+  </si>
+  <si>
+    <t>Se supone que solo se permite el registro de usuarios que están en la lista de la página.</t>
+  </si>
+  <si>
+    <t>Se supone que ya existen usuarios en la lista.</t>
+  </si>
+  <si>
+    <t>Se supone que los servicios de registro en la página están funcionales y estables.</t>
+  </si>
+  <si>
+    <t>Se supone que los servicios de ingreso en la página están funcionales y estables.</t>
+  </si>
+  <si>
+    <t>Funcionamiento de los microservicios de la pagina reqres.in.</t>
+  </si>
+  <si>
+    <t>Funcionamiento de los microservicios de la pagina tiendacereza.com.</t>
+  </si>
+  <si>
+    <t>Se recomienda ejecutar pruebas de seguridad.
+Se recomienda ejecutar pruebas de rendimiento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se probará la respuesta de la petición.
+Se probará el URL de la petición realizando cambios en los campos de correo "name.last@reqres.in" y contraseña "pass123".
+Se realizarán peticiones con diferentes estructuras en el cuerpo a enviar.
+</t>
   </si>
   <si>
     <r>
@@ -129,76 +507,15 @@
 3. Verificar que, al enviar un valor adecuado al parámetro, la respuesta sea aceptada.
 4. Verificar que, al enviar un valor inadecuado al parámetro, la respuesta sea fallida.</t>
     </r>
-  </si>
-  <si>
-    <t>Sprint</t>
-  </si>
-  <si>
-    <t>Abarca la ejecución de las pruebas funcionales para la petición GET LIST USERS en el canal: https://reqres.in</t>
-  </si>
-  <si>
-    <t>Abarca la ejecución de las pruebas funcionales para la petición POST REGISTER en el canal: https://reqres.in</t>
-  </si>
-  <si>
-    <t>Se probará el código de estado de respuesta de la petición.
-Se probará el URL de la petición realizando cambios en el parámetro de la página.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">No hace parte del alcance:
-</t>
-    </r>
     <r>
       <rPr>
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
-      <t>No es objeto de prueba la verificación de funcionalidades que no hagan parte de la petición GET LIST USERS.
-Tampoco se tendrá en cuenta pruebas de seguridad, rendimiento y estrés.</t>
-    </r>
-  </si>
-  <si>
-    <t>Las actividades descritas en el alcance se realizarán en el transcurso del 27 de febrero en las horas 11:00 AM a 12:00 PM.</t>
-  </si>
-  <si>
-    <t>Se recomienda ejecutar pruebas de seguridad.
-Se recomienda ejecutar pruebas de rendimiento.</t>
-  </si>
-  <si>
-    <t>Ya existen usuarios en la lista.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">No hace parte del alcance:
+      <t xml:space="preserve">
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>No es objeto de prueba la verificación de funcionalidades que no hagan parte de la petición POST REGISTER.
-Tampoco se tendrá en cuenta pruebas de seguridad, rendimiento y estrés.</t>
     </r>
   </si>
   <si>
@@ -222,217 +539,79 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1. Verificar que un usuario NO definido NO se puede registrar.
-2. Verificar la visualización del mensaje de error cuando el campo de contraseña está vacío.
-3. Verificar la visualización del mensaje de error cuando el campo de correo está vacío.
-4. Verificar que la contraseña contenga mínimo 8 caracteres.</t>
+      <t>1. Verificar que, al registrar un nuevo usuario, el sistema solicite de manera obligatoria el ingreso de la siguiente información: correo y contraseña.
+2. Verificar que, al registrar un nuevo usuario, el sistema solicite de manera NO obligatoria el ingreso de la siguiente información: nombre y apellido.
+3. Verificar la visualización del mensaje de error cuando se trata de crear un usuario con un correo ya existente en la BD del sistema.
+4. Verificar que la contraseña contenga mínimo 5 caracteres.</t>
     </r>
-  </si>
-  <si>
-    <t>N°</t>
-  </si>
-  <si>
-    <t>Identificador</t>
-  </si>
-  <si>
-    <t>Descripción</t>
-  </si>
-  <si>
-    <t>Pre-Condición</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entradas </t>
-  </si>
-  <si>
-    <t>Pasos Caso Prueba</t>
-  </si>
-  <si>
-    <t>Resultado Esperado</t>
-  </si>
-  <si>
-    <t>Resultado</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
-    <t>CA01</t>
-  </si>
-  <si>
-    <t>Verificar si la respuesta al realizar la petición adecuadamente es la correcta (200 OK).</t>
-  </si>
-  <si>
-    <t>La pagina https://reqres.in debe estar en funcionamiento.</t>
-  </si>
-  <si>
-    <t>Estando dentro del entorno descrito en el apartado de contexto de la sección Alcance:
-1. Ingresar a la aplicación Postman.
-2. Crear una nueva HTTP Request de tipo GET.
-3. Ingresar la URL https://reqres.in/api/users?page=2 a esta petición.
-4. Enviarla.
-5. Revisar si la respuesta es la correcta.</t>
-  </si>
-  <si>
-    <t>Recibir una respuesta con el STATUS: 200 OK.</t>
-  </si>
-  <si>
-    <t>Pasó</t>
-  </si>
-  <si>
-    <t>Terminado</t>
-  </si>
-  <si>
-    <t>CA02</t>
-  </si>
-  <si>
-    <t>Verificar que el contenido de la respuesta corresponda al formato adecuado (JSON).</t>
-  </si>
-  <si>
-    <t>Estando dentro del entorno descrito en el apartado de contexto de la sección Alcance:
-1. Identificar los parámetros de la solicitud de la API.
-2. Ingresar a la aplicación Postman.
-3. Crear una nueva HTTP Request de tipo GET.
-4. Ingresar la URL https://reqres.in/api/users?page=2 a esta petición.
-5. Enviarla.
-6. Revisar que el cuerpo de la respuesta de la petición sea el correspondiente en el formato JSON.</t>
-  </si>
-  <si>
-    <t>Recibir una respuesta en formato JSON, así:
-{
-    "id": 1,
-    "email": "email@email.com",
-    "first_name": "nombre",
-    "last_name": "apellido",
-    "avatar": "imange.jpg"
- }</t>
-  </si>
-  <si>
-    <t>CA03</t>
-  </si>
-  <si>
-    <t>Verificar que al enviar un valor adecuado al parámetro, la respuesta sea aceptada.</t>
-  </si>
-  <si>
-    <t>Estando dentro del entorno descrito en el apartado de contexto de la sección Alcance:
-1. Ingresar a la aplicación Postman.
-2. Crear una nueva HTTP Request de tipo GET.
-3. Ingresar la URL https://reqres.in/api/users?page=2 a esta petición.
-4. Enviarla.
-5. Revisar si la respuesta a la petición es la correcta.</t>
-  </si>
-  <si>
-    <t>Recibir respuesta a la petición con el body indicado.</t>
-  </si>
-  <si>
-    <t>CA04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verificar que al enviar un valor inadecuado al parámetro, la respuesta sea fallida. </t>
-  </si>
-  <si>
-    <t>Estando dentro del entorno descrito en el apartado de contexto de la sección Alcance:
-1. Ingresar a la aplicación Postman.
-2. Crear una nueva HTTP Request de tipo GET.
-3. Ingresar la URL https://reqres.in/api/users?page=%!"@#;¨^.
-4. Enviarla.
-5. Revisar si la respuesta a la petición es fallida.</t>
-  </si>
-  <si>
-    <t>Recibir una respuesta fallida a la petición.</t>
-  </si>
-  <si>
-    <t>No pasó</t>
-  </si>
-  <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
-    <t>Impacto</t>
-  </si>
-  <si>
-    <t>Tipo</t>
-  </si>
-  <si>
-    <t>Probabilidad de ocurrencia</t>
-  </si>
-  <si>
-    <t>Severidad</t>
-  </si>
-  <si>
-    <t>Nivel de riesgo</t>
-  </si>
-  <si>
-    <t>Acción</t>
-  </si>
-  <si>
-    <t>Plan de Acción</t>
-  </si>
-  <si>
-    <t>Mala determinación del tipo de respuesta HTTP.</t>
-  </si>
-  <si>
-    <t>Producto</t>
-  </si>
-  <si>
-    <t>Ignorar</t>
-  </si>
-  <si>
-    <t>Revisión y validación de la respuesta HTTP antes de permitir recibir peticiones.</t>
-  </si>
-  <si>
-    <t>Estructura JSON con formato erróneo.</t>
-  </si>
-  <si>
-    <t>Mitigar</t>
-  </si>
-  <si>
-    <t>Reestructurar el JSON a ser entregado de la manera correcta.</t>
-  </si>
-  <si>
-    <t>La petición no es aceptada a pesar de enviar un valor de parámetro correcto.</t>
-  </si>
-  <si>
-    <t>Contener</t>
-  </si>
-  <si>
-    <t>Revisar el codigo detrás de la petición y cambiar la parte de validación del parametro recibido.</t>
-  </si>
-  <si>
-    <t>La petición es aceptada a pesar de enviar un valor de parámetro incorrecto.</t>
-  </si>
-  <si>
-    <t>Un usuario que está definido, no se puede registrar.</t>
-  </si>
-  <si>
-    <t>Realizar una correcta asociación entre la definición de usuario y el sistema de registro.</t>
-  </si>
-  <si>
-    <t>Se registra un usuario con contraseña vacía.</t>
-  </si>
-  <si>
-    <t>Realizar una correcta definición de las reglas para la aceptación de una contraseña como válida.</t>
-  </si>
-  <si>
-    <t>Se registra un usuario con correo vacío.</t>
-  </si>
-  <si>
-    <t>Realizar una correcta definición de las reglas para la aceptación de un correo como válido.</t>
-  </si>
-  <si>
-    <t>Se registra un usuario con contraseña de menos de 5 caracteres.</t>
-  </si>
-  <si>
-    <t>Transferir</t>
-  </si>
-  <si>
-    <t>Informar del defecto al equipo de desarrollo.</t>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Hace parte del alcance:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1. Verificar la visualización del mensaje de error al intentar ingresar sin rellenar el campo de contraseña.
+2. Verificar la visualización del mensaje de error al intentar ingresar sin rellenar el campo de correo.
+3. Verificar la visualización del mensaje de error al intentar ingresar con un usuario no registrado.
+4. Verificar la visualización del mensaje de error al intentar ingresar con una contraseña incorrecta para el usuario especificado.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Se recomienda ejecutar pruebas de seguridad.
+Se recomienda ejecutar pruebas de rendimiento.
+Se recomienda ejecutar pruebas de estrés.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se probará que se exijan campos mínimos para el registro.
+Se realizaran registros con diferentes combinaciones de correo y contraseña, ya sean existentes o no, con longitudes de contraseña variantes.
+</t>
+  </si>
+  <si>
+    <t>Se probará el ingreso de usuarios que se hayan creado y usuarios que no se sepa de su existencia en la BD de la página.
+Se realizarán ingresos de usuario con los campos vacíos de correo o contraseña.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,8 +653,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,11 +696,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FFD8D8D8"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -542,98 +735,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFFF7E06"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFF7E06"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFF7E06"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFF7E06"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -695,11 +796,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF7E06"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF7E06"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF7E06"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -725,49 +839,44 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1099,6 +1208,7 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFA5A5A5"/>
       <color rgb="FFFF7E06"/>
     </mruColors>
   </colors>
@@ -1288,16 +1398,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>192676</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>305889</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>148561</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1569720</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>333618</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1319349</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1327,8 +1437,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7932420" y="647700"/>
-          <a:ext cx="6480781" cy="3299460"/>
+          <a:off x="9728562" y="1448889"/>
+          <a:ext cx="6498199" cy="3299460"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1359,6 +1469,7 @@
     <sheetNames>
       <sheetName val="Matriz de Riesgo"/>
       <sheetName val="Tabla"/>
+      <sheetName val="MatrizDeRiesgos"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -1428,6 +1539,7 @@
         </row>
       </sheetData>
       <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1732,179 +1844,185 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EA6F44-0A13-4B3B-95DA-2DE7B9084CBB}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" topLeftCell="L1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" style="5" customWidth="1"/>
-    <col min="6" max="6" width="33.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="69.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="43.33203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="34" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.44140625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="34.33203125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="30.88671875" style="5" customWidth="1"/>
-    <col min="13" max="13" width="22.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="5" customWidth="1"/>
+    <col min="6" max="6" width="33.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="74" style="5" customWidth="1"/>
+    <col min="8" max="8" width="45.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.6640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="33.21875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="29.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="11.44140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="11"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="14"/>
-    </row>
-    <row r="3" spans="1:13" ht="36" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+    </row>
+    <row r="3" spans="1:13" s="16" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="180" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="162" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="162" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="126" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="J5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="L5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="J1:M1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1915,102 +2033,186 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52918882-42F7-4A79-8BF7-71EFDDF0321F}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="81.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.33203125" customWidth="1"/>
+    <col min="13" max="13" width="29.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="11"/>
-    </row>
-    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="14"/>
-    </row>
-    <row r="3" spans="1:13" ht="306" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+    </row>
+    <row r="2" spans="1:13" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+    </row>
+    <row r="3" spans="1:13" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="162" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="E4" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="180" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" ht="306" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+      <c r="F5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="J1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2021,310 +2223,310 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480FDED1-1A1E-44D7-B872-85FF24D4C5DB}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:J10"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="A2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="17" t="s">
+    </row>
+    <row r="3" spans="1:10" ht="180" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="17" t="s">
+      <c r="C3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="180" x14ac:dyDescent="0.3">
-      <c r="A3" s="22">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11">
+        <v>3</v>
+      </c>
+      <c r="F3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22">
-        <v>3</v>
-      </c>
-      <c r="F3" s="22">
-        <v>1</v>
-      </c>
-      <c r="G3" s="23">
+      <c r="G3" s="12">
         <f>'[1]Matriz de Riesgo'!$E3*'[1]Matriz de Riesgo'!$F3</f>
         <v>3</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="12">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
         <v>3</v>
       </c>
-      <c r="I3" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="J3" s="22" t="s">
-        <v>70</v>
+      <c r="I3" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="A4" s="22">
+      <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22">
+      <c r="B4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11">
         <v>1</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="11">
         <v>5</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="12">
         <f>'[1]Matriz de Riesgo'!$E4*'[1]Matriz de Riesgo'!$F4</f>
         <v>5</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="12">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
         <v>5</v>
       </c>
-      <c r="I4" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>73</v>
+      <c r="I4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="234" x14ac:dyDescent="0.3">
-      <c r="A5" s="22">
+      <c r="A5" s="11">
         <v>3</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22">
+      <c r="B5" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11">
         <v>1</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="11">
         <v>5</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="12">
         <f>'[1]Matriz de Riesgo'!$E5*'[1]Matriz de Riesgo'!$F5</f>
         <v>5</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="12">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
         <v>5</v>
       </c>
-      <c r="I5" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>76</v>
+      <c r="I5" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="234" x14ac:dyDescent="0.3">
-      <c r="A6" s="22">
+      <c r="A6" s="11">
         <v>4</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22">
+      <c r="B6" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11">
         <v>5</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="11">
         <v>5</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="12">
         <f>'[1]Matriz de Riesgo'!$E6*'[1]Matriz de Riesgo'!$F6</f>
         <v>25</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="12">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
         <v>25</v>
       </c>
-      <c r="I6" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>76</v>
+      <c r="I6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="198" x14ac:dyDescent="0.3">
-      <c r="A7" s="22">
+      <c r="A7" s="11">
         <v>1</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22">
+      <c r="B7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11">
         <v>3</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="11">
         <v>5</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="12">
         <f>'[1]Matriz de Riesgo'!$E7*'[1]Matriz de Riesgo'!$F7</f>
         <v>15</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="12">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
         <v>15</v>
       </c>
-      <c r="I7" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>79</v>
+      <c r="I7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="A8" s="22">
+      <c r="A8" s="11">
         <v>2</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22">
+      <c r="B8" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11">
         <v>1</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="11">
         <v>5</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="12">
         <f>'[1]Matriz de Riesgo'!$E8*'[1]Matriz de Riesgo'!$F8</f>
         <v>5</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="12">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
         <v>5</v>
       </c>
-      <c r="I8" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>81</v>
+      <c r="I8" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="A9" s="22">
+      <c r="A9" s="11">
         <v>3</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22">
+      <c r="B9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11">
         <v>1</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="11">
         <v>5</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="12">
         <f>'[1]Matriz de Riesgo'!$E9*'[1]Matriz de Riesgo'!$F9</f>
         <v>5</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="12">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
         <v>5</v>
       </c>
-      <c r="I9" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="J9" s="22" t="s">
-        <v>83</v>
+      <c r="I9" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="198" x14ac:dyDescent="0.3">
-      <c r="A10" s="22">
+      <c r="A10" s="11">
         <v>4</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22">
+      <c r="B10" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11">
         <v>5</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="11">
         <v>2</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="12">
         <f>'[1]Matriz de Riesgo'!$E10*'[1]Matriz de Riesgo'!$F10</f>
         <v>10</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="12">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
         <v>10</v>
       </c>
-      <c r="I10" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="J10" s="22" t="s">
-        <v>86</v>
+      <c r="I10" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2340,310 +2542,310 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9E30F7-763E-44A1-AC72-B58C102A0249}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="A2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="17" t="s">
+    </row>
+    <row r="3" spans="1:10" ht="180" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="17" t="s">
+      <c r="C3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="180" x14ac:dyDescent="0.3">
-      <c r="A3" s="22">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11">
+        <v>3</v>
+      </c>
+      <c r="F3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22">
-        <v>3</v>
-      </c>
-      <c r="F3" s="22">
-        <v>1</v>
-      </c>
-      <c r="G3" s="23">
+      <c r="G3" s="12">
         <f>'[1]Matriz de Riesgo'!$E3*'[1]Matriz de Riesgo'!$F3</f>
         <v>3</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="12" t="e">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>3</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="J3" s="22" t="s">
-        <v>70</v>
+        <v>#REF!</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="A4" s="22">
+      <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22">
+      <c r="B4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11">
         <v>1</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="11">
         <v>5</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="12">
         <f>'[1]Matriz de Riesgo'!$E4*'[1]Matriz de Riesgo'!$F4</f>
         <v>5</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="12" t="e">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="234" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11">
         <v>5</v>
       </c>
-      <c r="I4" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="234" x14ac:dyDescent="0.3">
-      <c r="A5" s="22">
-        <v>3</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22">
-        <v>1</v>
-      </c>
-      <c r="F5" s="22">
-        <v>5</v>
-      </c>
-      <c r="G5" s="23">
+      <c r="G5" s="12">
         <f>'[1]Matriz de Riesgo'!$E5*'[1]Matriz de Riesgo'!$F5</f>
         <v>5</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="12" t="e">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="234" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11">
         <v>5</v>
       </c>
-      <c r="I5" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="234" x14ac:dyDescent="0.3">
-      <c r="A6" s="22">
-        <v>4</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22">
+      <c r="F6" s="11">
         <v>5</v>
       </c>
-      <c r="F6" s="22">
-        <v>5</v>
-      </c>
-      <c r="G6" s="23">
+      <c r="G6" s="12">
         <f>'[1]Matriz de Riesgo'!$E6*'[1]Matriz de Riesgo'!$F6</f>
         <v>25</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="12" t="e">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>25</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>76</v>
+        <v>#REF!</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="198" x14ac:dyDescent="0.3">
-      <c r="A7" s="22">
+      <c r="A7" s="11">
         <v>1</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22">
+      <c r="B7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11">
         <v>3</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="11">
         <v>5</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="12">
         <f>'[1]Matriz de Riesgo'!$E7*'[1]Matriz de Riesgo'!$F7</f>
         <v>15</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="12" t="e">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>15</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>79</v>
+        <v>#REF!</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="A8" s="22">
+      <c r="A8" s="11">
         <v>2</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22">
+      <c r="B8" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11">
         <v>1</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="11">
         <v>5</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="12">
         <f>'[1]Matriz de Riesgo'!$E8*'[1]Matriz de Riesgo'!$F8</f>
         <v>5</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="12" t="e">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>3</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11">
         <v>5</v>
       </c>
-      <c r="I8" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="A9" s="22">
-        <v>3</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22">
-        <v>1</v>
-      </c>
-      <c r="F9" s="22">
-        <v>5</v>
-      </c>
-      <c r="G9" s="23">
+      <c r="G9" s="12">
         <f>'[1]Matriz de Riesgo'!$E9*'[1]Matriz de Riesgo'!$F9</f>
         <v>5</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="12" t="e">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="198" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>4</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11">
         <v>5</v>
       </c>
-      <c r="I9" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="J9" s="22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="198" x14ac:dyDescent="0.3">
-      <c r="A10" s="22">
-        <v>4</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22">
-        <v>5</v>
-      </c>
-      <c r="F10" s="22">
+      <c r="F10" s="11">
         <v>2</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="12">
         <f>'[1]Matriz de Riesgo'!$E10*'[1]Matriz de Riesgo'!$F10</f>
         <v>10</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="12" t="e">
         <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>10</v>
-      </c>
-      <c r="I10" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="J10" s="22" t="s">
-        <v>86</v>
+        <v>#REF!</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2659,50 +2861,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF64FDF5-5E03-4C8A-948F-964343A0E4F3}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
       <selection sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" ht="54" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="G2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="I2" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
@@ -2710,26 +2912,26 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
@@ -2737,26 +2939,26 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
@@ -2764,26 +2966,26 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
@@ -2791,26 +2993,26 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2825,8 +3027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2406D1D5-C0F8-4862-8277-1721ED58A928}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2839,7 +3041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FCE272-65CE-4E61-8DFF-1708BEA28DC8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
✨ Adding traditional test case
</commit_message>
<xml_diff>
--- a/PlanDePruebasRiesgosCasosDePrueba.xlsx
+++ b/PlanDePruebasRiesgosCasosDePrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\Training\Duras\Repos\C1-2023-QA-Calidad-T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DCCA6A-27A7-4526-A842-9F4322670DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7ABCA4-40A4-4264-BD2C-711FE1C9B9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
   </bookViews>
   <sheets>
     <sheet name="PlaneDePruebaServicios" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
     <sheet name="CPServicioPOST" sheetId="4" r:id="rId6"/>
     <sheet name="CPLoginRegistroTiendaCereza" sheetId="5" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="106">
   <si>
     <t>Célula</t>
   </si>
@@ -215,9 +212,6 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>CA01</t>
-  </si>
-  <si>
     <t>Verificar si la respuesta al realizar la petición adecuadamente es la correcta (200 OK).</t>
   </si>
   <si>
@@ -236,12 +230,6 @@
   </si>
   <si>
     <t>Pasó</t>
-  </si>
-  <si>
-    <t>Terminado</t>
-  </si>
-  <si>
-    <t>CA02</t>
   </si>
   <si>
     <t>Verificar que el contenido de la respuesta corresponda al formato adecuado (JSON).</t>
@@ -256,19 +244,6 @@
 6. Revisar que el cuerpo de la respuesta de la petición sea el correspondiente en el formato JSON.</t>
   </si>
   <si>
-    <t>Recibir una respuesta en formato JSON, así:
-{
-    "id": 1,
-    "email": "email@email.com",
-    "first_name": "nombre",
-    "last_name": "apellido",
-    "avatar": "imange.jpg"
- }</t>
-  </si>
-  <si>
-    <t>CA03</t>
-  </si>
-  <si>
     <t>Verificar que al enviar un valor adecuado al parámetro, la respuesta sea aceptada.</t>
   </si>
   <si>
@@ -283,9 +258,6 @@
     <t>Recibir respuesta a la petición con el body indicado.</t>
   </si>
   <si>
-    <t>CA04</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verificar que al enviar un valor inadecuado al parámetro, la respuesta sea fallida. </t>
   </si>
   <si>
@@ -301,9 +273,6 @@
   </si>
   <si>
     <t>No pasó</t>
-  </si>
-  <si>
-    <t>Pendiente</t>
   </si>
   <si>
     <t>Impacto</t>
@@ -428,30 +397,6 @@
   </si>
   <si>
     <t>Las actividades descritas en el alcance se realizarán en el transcurso del 27 de febrero en las horas 03:30 PM a 04:25 PM.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">No hace parte del alcance:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>No es objeto de prueba la verificación de funcionalidades que no hagan parte del sistema de resgistro en la Tienda Cereza 🍒.
-Tampoco se tendrá en cuenta pruebas de seguridad, rendimiento y estrés.</t>
-    </r>
   </si>
   <si>
     <t>Se supone que solo se permite el registro de usuarios que están en la lista de la página.</t>
@@ -605,6 +550,120 @@
   <si>
     <t>Se probará el ingreso de usuarios que se hayan creado y usuarios que no se sepa de su existencia en la BD de la página.
 Se realizarán ingresos de usuario con los campos vacíos de correo o contraseña.</t>
+  </si>
+  <si>
+    <t>CP01</t>
+  </si>
+  <si>
+    <t>CP02</t>
+  </si>
+  <si>
+    <t>CP03</t>
+  </si>
+  <si>
+    <t>CP04</t>
+  </si>
+  <si>
+    <t>Número de página a consultar como parametro</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">No hace parte del alcance:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No es objeto de prueba la verificación de funcionalidades que no hagan parte del sistema de registro en la Tienda Cereza 🍒.
+Tampoco se tendrá en cuenta pruebas de seguridad, rendimiento y estrés.</t>
+    </r>
+  </si>
+  <si>
+    <t>Se recibió una respuesta con el STATUS: 200 OK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Recibir una respuesta en formato JSON, así:
+{
+    "page": 2,
+    "per_page": 6,
+    "total": 1,
+    "total_pages": 2,
+    "data": [
+        {
+            "id": 7,
+            "email": "nombre.last@reqres.in",
+            "first_name": "Nombre",
+            "last_name": "Last",
+            "avatar": "image.jpg"
+        },
+    ],
+    "support": {
+        "url": "https://reqres.in/#support-heading",
+        "text": "Help!"
+    }
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Se recibió una respuesta en formato JSON, así:
+{
+    "page": 2,
+    "per_page": 6,
+    "total": 1,
+    "total_pages": 2,
+    "data": [
+        {
+            "id": 7,
+            "email": "nombre.last@reqres.in",
+            "first_name": "Nombre",
+            "last_name": "Last",
+            "avatar": "image.jpg"
+        },
+    ],
+    "support": {
+        "url": "https://reqres.in/#support-heading",
+        "text": "Help!"
+    }
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Se recibió una respuesta en formato JSON, así:
+{
+    "page": 1,
+    "per_page": 6,
+    "total": 1,
+    "total_pages": 2,
+    "data": [
+        {
+            "id": 7,
+            "email": "nombre.last@reqres.in",
+            "first_name": "Nombre",
+            "last_name": "Last",
+            "avatar": "image.jpg"
+        },
+    ],
+    "support": {
+        "url": "https://reqres.in/#support-heading",
+        "text": "Help!"
+    }
+}
+</t>
   </si>
 </sst>
 </file>
@@ -706,7 +765,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -785,19 +844,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFFF7E06"/>
       </left>
       <right style="thin">
@@ -813,7 +859,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -830,29 +876,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -861,10 +889,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -876,8 +904,20 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1333,15 +1373,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>38099</xdr:colOff>
+      <xdr:colOff>473528</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>495300</xdr:rowOff>
+      <xdr:rowOff>27215</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>179040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>594360</xdr:rowOff>
+      <xdr:colOff>614469</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>812075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1371,8 +1411,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8755379" y="723900"/>
-          <a:ext cx="6480781" cy="3299460"/>
+          <a:off x="11522528" y="255815"/>
+          <a:ext cx="6498198" cy="3299460"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1398,16 +1438,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>192676</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>305889</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>551904</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>153489</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>333618</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>1319349</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>692846</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>709749</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1437,7 +1477,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9728562" y="1448889"/>
+          <a:off x="11742418" y="382089"/>
           <a:ext cx="6498199" cy="3299460"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1458,91 +1498,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Matriz de Riesgo"/>
-      <sheetName val="Tabla"/>
-      <sheetName val="MatrizDeRiesgos"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="E3">
-            <v>3</v>
-          </cell>
-          <cell r="F3">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="E4">
-            <v>1</v>
-          </cell>
-          <cell r="F4">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="E5">
-            <v>1</v>
-          </cell>
-          <cell r="F5">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="E6">
-            <v>5</v>
-          </cell>
-          <cell r="F6">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="E7">
-            <v>3</v>
-          </cell>
-          <cell r="F7">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="E8">
-            <v>1</v>
-          </cell>
-          <cell r="F8">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="E9">
-            <v>1</v>
-          </cell>
-          <cell r="F9">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>5</v>
-          </cell>
-          <cell r="F10">
-            <v>2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1844,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EA6F44-0A13-4B3B-95DA-2DE7B9084CBB}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="L1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:M5"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -1867,115 +1822,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-    </row>
-    <row r="3" spans="1:13" s="16" customFormat="1" ht="36" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+    </row>
+    <row r="3" spans="1:13" s="10" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="19" t="s">
+      <c r="G3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="M3" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="180" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="H4" s="17" t="s">
+      <c r="G4" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="J4" s="17" t="s">
+      <c r="I4" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>91</v>
+      <c r="K4" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="162" x14ac:dyDescent="0.3">
@@ -2004,25 +1959,25 @@
         <v>23</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="L5" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2035,8 +1990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52918882-42F7-4A79-8BF7-71EFDDF0321F}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2057,115 +2012,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-    </row>
-    <row r="3" spans="1:13" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+    </row>
+    <row r="3" spans="1:13" s="9" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="19" t="s">
+      <c r="G3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="M3" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="162" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="J4" s="17" t="s">
+      <c r="F4" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="K4" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>92</v>
+      <c r="L4" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="180" x14ac:dyDescent="0.3">
@@ -2185,34 +2140,34 @@
         <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2223,316 +2178,354 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480FDED1-1A1E-44D7-B872-85FF24D4C5DB}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.5546875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="20"/>
+    <col min="5" max="5" width="16" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="20"/>
+    <col min="8" max="8" width="10.5546875" style="20" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.5546875" style="20"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-    </row>
-    <row r="2" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" ht="36" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <f>E3*F3</f>
+        <v>3</v>
+      </c>
+      <c r="H3" s="1">
+        <f>G3</f>
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="J3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H2" s="7" t="s">
+    </row>
+    <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="C4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" ref="G4:G10" si="0">E4*F4</f>
+        <v>5</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" ref="H4:H10" si="1">G4</f>
+        <v>5</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J4" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="180" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11">
+      <c r="J5" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
         <v>3</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="12">
-        <f>'[1]Matriz de Riesgo'!$E3*'[1]Matriz de Riesgo'!$F3</f>
-        <v>3</v>
-      </c>
-      <c r="H3" s="12">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>3</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11">
-        <v>1</v>
-      </c>
-      <c r="F4" s="11">
-        <v>5</v>
-      </c>
-      <c r="G4" s="12">
-        <f>'[1]Matriz de Riesgo'!$E4*'[1]Matriz de Riesgo'!$F4</f>
-        <v>5</v>
-      </c>
-      <c r="H4" s="12">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>5</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="234" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11">
-        <v>1</v>
-      </c>
-      <c r="F5" s="11">
-        <v>5</v>
-      </c>
-      <c r="G5" s="12">
-        <f>'[1]Matriz de Riesgo'!$E5*'[1]Matriz de Riesgo'!$F5</f>
-        <v>5</v>
-      </c>
-      <c r="H5" s="12">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>5</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="234" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11">
-        <v>5</v>
-      </c>
-      <c r="F6" s="11">
-        <v>5</v>
-      </c>
-      <c r="G6" s="12">
-        <f>'[1]Matriz de Riesgo'!$E6*'[1]Matriz de Riesgo'!$F6</f>
-        <v>25</v>
-      </c>
-      <c r="H6" s="12">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>25</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="198" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
-        <v>1</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="G10" s="4">
+        <f>E10*F10</f>
+        <v>10</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11">
-        <v>3</v>
-      </c>
-      <c r="F7" s="11">
-        <v>5</v>
-      </c>
-      <c r="G7" s="12">
-        <f>'[1]Matriz de Riesgo'!$E7*'[1]Matriz de Riesgo'!$F7</f>
-        <v>15</v>
-      </c>
-      <c r="H7" s="12">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>15</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" s="11" t="s">
+      <c r="J10" s="3" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
-        <v>2</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11">
-        <v>1</v>
-      </c>
-      <c r="F8" s="11">
-        <v>5</v>
-      </c>
-      <c r="G8" s="12">
-        <f>'[1]Matriz de Riesgo'!$E8*'[1]Matriz de Riesgo'!$F8</f>
-        <v>5</v>
-      </c>
-      <c r="H8" s="12">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>5</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
-        <v>3</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11">
-        <v>1</v>
-      </c>
-      <c r="F9" s="11">
-        <v>5</v>
-      </c>
-      <c r="G9" s="12">
-        <f>'[1]Matriz de Riesgo'!$E9*'[1]Matriz de Riesgo'!$F9</f>
-        <v>5</v>
-      </c>
-      <c r="H9" s="12">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>5</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="198" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
-        <v>4</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11">
-        <v>5</v>
-      </c>
-      <c r="F10" s="11">
-        <v>2</v>
-      </c>
-      <c r="G10" s="12">
-        <f>'[1]Matriz de Riesgo'!$E10*'[1]Matriz de Riesgo'!$F10</f>
-        <v>10</v>
-      </c>
-      <c r="H10" s="12">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>10</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
+  <conditionalFormatting sqref="H3:H10">
+    <cfRule type="iconSet" priority="1">
+      <iconSet showValue="0" reverse="1">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="4"/>
+        <cfvo type="num" val="12"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2543,315 +2536,353 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:J10"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.21875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="20"/>
+    <col min="5" max="5" width="16" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="20"/>
+    <col min="8" max="8" width="10.5546875" style="20" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.21875" style="20" customWidth="1"/>
+    <col min="11" max="16384" width="11.5546875" style="20"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-    </row>
-    <row r="2" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" ht="36" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <f>E3*F3</f>
+        <v>3</v>
+      </c>
+      <c r="H3" s="1">
+        <f>G3</f>
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="J3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H2" s="7" t="s">
+    </row>
+    <row r="4" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="C4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" ref="G4:G10" si="0">E4*F4</f>
+        <v>5</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" ref="H4:H10" si="1">G4</f>
+        <v>5</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J4" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="180" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11">
+      <c r="J5" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4">
+        <f>E6*F6</f>
+        <v>25</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
         <v>3</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="12">
-        <f>'[1]Matriz de Riesgo'!$E3*'[1]Matriz de Riesgo'!$F3</f>
-        <v>3</v>
-      </c>
-      <c r="H3" s="12" t="e">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="144" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11">
-        <v>1</v>
-      </c>
-      <c r="F4" s="11">
-        <v>5</v>
-      </c>
-      <c r="G4" s="12">
-        <f>'[1]Matriz de Riesgo'!$E4*'[1]Matriz de Riesgo'!$F4</f>
-        <v>5</v>
-      </c>
-      <c r="H4" s="12" t="e">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="234" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11">
-        <v>1</v>
-      </c>
-      <c r="F5" s="11">
-        <v>5</v>
-      </c>
-      <c r="G5" s="12">
-        <f>'[1]Matriz de Riesgo'!$E5*'[1]Matriz de Riesgo'!$F5</f>
-        <v>5</v>
-      </c>
-      <c r="H5" s="12" t="e">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="234" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11">
-        <v>5</v>
-      </c>
-      <c r="F6" s="11">
-        <v>5</v>
-      </c>
-      <c r="G6" s="12">
-        <f>'[1]Matriz de Riesgo'!$E6*'[1]Matriz de Riesgo'!$F6</f>
-        <v>25</v>
-      </c>
-      <c r="H6" s="12" t="e">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="198" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
-        <v>1</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11">
-        <v>3</v>
-      </c>
-      <c r="F7" s="11">
-        <v>5</v>
-      </c>
-      <c r="G7" s="12">
-        <f>'[1]Matriz de Riesgo'!$E7*'[1]Matriz de Riesgo'!$F7</f>
-        <v>15</v>
-      </c>
-      <c r="H7" s="12" t="e">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" s="11" t="s">
+      <c r="J10" s="3" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
-        <v>2</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11">
-        <v>1</v>
-      </c>
-      <c r="F8" s="11">
-        <v>5</v>
-      </c>
-      <c r="G8" s="12">
-        <f>'[1]Matriz de Riesgo'!$E8*'[1]Matriz de Riesgo'!$F8</f>
-        <v>5</v>
-      </c>
-      <c r="H8" s="12" t="e">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="216" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
-        <v>3</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11">
-        <v>1</v>
-      </c>
-      <c r="F9" s="11">
-        <v>5</v>
-      </c>
-      <c r="G9" s="12">
-        <f>'[1]Matriz de Riesgo'!$E9*'[1]Matriz de Riesgo'!$F9</f>
-        <v>5</v>
-      </c>
-      <c r="H9" s="12" t="e">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="198" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
-        <v>4</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11">
-        <v>5</v>
-      </c>
-      <c r="F10" s="11">
-        <v>2</v>
-      </c>
-      <c r="G10" s="12">
-        <f>'[1]Matriz de Riesgo'!$E10*'[1]Matriz de Riesgo'!$F10</f>
-        <v>10</v>
-      </c>
-      <c r="H10" s="12" t="e">
-        <f>[1]!Table_1[[#This Row],[Severidad]]</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
+  <conditionalFormatting sqref="H3:H10">
+    <cfRule type="iconSet" priority="1">
+      <iconSet showValue="0" reverse="1">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="4"/>
+        <cfvo type="num" val="12"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2861,158 +2892,177 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF64FDF5-5E03-4C8A-948F-964343A0E4F3}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection sqref="A1:I6"/>
+    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="78" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.21875" customWidth="1"/>
+    <col min="8" max="8" width="54.88671875" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-    </row>
-    <row r="2" spans="1:9" ht="54" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="126" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" ht="396" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="F4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="126" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="F5" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="396" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="F6" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
✨ Adding Gherkin test cases for post service and for Tienda Cereza
</commit_message>
<xml_diff>
--- a/PlanDePruebasRiesgosCasosDePrueba.xlsx
+++ b/PlanDePruebasRiesgosCasosDePrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\Training\Duras\Repos\C1-2023-QA-Calidad-T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7ABCA4-40A4-4264-BD2C-711FE1C9B9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31CEAFC-924F-40CA-87DB-FDE58C652999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="5" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
   </bookViews>
   <sheets>
     <sheet name="PlaneDePruebaServicios" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="195">
   <si>
     <t>Célula</t>
   </si>
@@ -244,9 +244,6 @@
 6. Revisar que el cuerpo de la respuesta de la petición sea el correspondiente en el formato JSON.</t>
   </si>
   <si>
-    <t>Verificar que al enviar un valor adecuado al parámetro, la respuesta sea aceptada.</t>
-  </si>
-  <si>
     <t>Estando dentro del entorno descrito en el apartado de contexto de la sección Alcance:
 1. Ingresar a la aplicación Postman.
 2. Crear una nueva HTTP Request de tipo GET.
@@ -258,18 +255,12 @@
     <t>Recibir respuesta a la petición con el body indicado.</t>
   </si>
   <si>
-    <t xml:space="preserve">Verificar que al enviar un valor inadecuado al parámetro, la respuesta sea fallida. </t>
-  </si>
-  <si>
     <t>Estando dentro del entorno descrito en el apartado de contexto de la sección Alcance:
 1. Ingresar a la aplicación Postman.
 2. Crear una nueva HTTP Request de tipo GET.
 3. Ingresar la URL https://reqres.in/api/users?page=%!"@#;¨^.
 4. Enviarla.
 5. Revisar si la respuesta a la petición es fallida.</t>
-  </si>
-  <si>
-    <t>Recibir una respuesta fallida a la petición.</t>
   </si>
   <si>
     <t>No pasó</t>
@@ -501,6 +492,344 @@
     </r>
   </si>
   <si>
+    <t>Se recomienda ejecutar pruebas de seguridad.
+Se recomienda ejecutar pruebas de rendimiento.
+Se recomienda ejecutar pruebas de estrés.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se probará que se exijan campos mínimos para el registro.
+Se realizaran registros con diferentes combinaciones de correo y contraseña, ya sean existentes o no, con longitudes de contraseña variantes.
+</t>
+  </si>
+  <si>
+    <t>Se probará el ingreso de usuarios que se hayan creado y usuarios que no se sepa de su existencia en la BD de la página.
+Se realizarán ingresos de usuario con los campos vacíos de correo o contraseña.</t>
+  </si>
+  <si>
+    <t>CP01</t>
+  </si>
+  <si>
+    <t>CP02</t>
+  </si>
+  <si>
+    <t>CP03</t>
+  </si>
+  <si>
+    <t>CP04</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">No hace parte del alcance:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No es objeto de prueba la verificación de funcionalidades que no hagan parte del sistema de registro en la Tienda Cereza 🍒.
+Tampoco se tendrá en cuenta pruebas de seguridad, rendimiento y estrés.</t>
+    </r>
+  </si>
+  <si>
+    <t>Se recibió una respuesta con el STATUS: 200 OK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Recibir una respuesta en formato JSON, así:
+{
+    "page": 2,
+    "per_page": 6,
+    "total": 1,
+    "total_pages": 2,
+    "data": [
+        {
+            "id": 7,
+            "email": "nombre.last@reqres.in",
+            "first_name": "Nombre",
+            "last_name": "Last",
+            "avatar": "image.jpg"
+        },
+    ],
+    "support": {
+        "url": "https://reqres.in/#support-heading",
+        "text": "Help!"
+    }
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Se recibió una respuesta en formato JSON, así:
+{
+    "page": 2,
+    "per_page": 6,
+    "total": 1,
+    "total_pages": 2,
+    "data": [
+        {
+            "id": 7,
+            "email": "nombre.last@reqres.in",
+            "first_name": "Nombre",
+            "last_name": "Last",
+            "avatar": "image.jpg"
+        },
+    ],
+    "support": {
+        "url": "https://reqres.in/#support-heading",
+        "text": "Help!"
+    }
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Se recibió una respuesta en formato JSON, así:
+{
+    "page": 1,
+    "per_page": 6,
+    "total": 1,
+    "total_pages": 2,
+    "data": [
+        {
+            "id": 7,
+            "email": "nombre.last@reqres.in",
+            "first_name": "Nombre",
+            "last_name": "Last",
+            "avatar": "image.jpg"
+        },
+    ],
+    "support": {
+        "url": "https://reqres.in/#support-heading",
+        "text": "Help!"
+    }
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificar que al enviar un valor inadecuado al parámetro (page=), la respuesta sea fallida. </t>
+  </si>
+  <si>
+    <t>Verificar que al enviar un valor adecuado al parámetro (page=2), el contenido del cuerpo de respuesta sea el correspondiente.</t>
+  </si>
+  <si>
+    <t>Listas de Usuarios</t>
+  </si>
+  <si>
+    <t>Escenario:</t>
+  </si>
+  <si>
+    <t>Número de página a consultar como parámetro.</t>
+  </si>
+  <si>
+    <t>Recibir una respuesta fallida a la petición con un mensaje de error informando que el parámetro es inadecuado.</t>
+  </si>
+  <si>
+    <t>Metodo Gherkin:</t>
+  </si>
+  <si>
+    <t>POST REGISTER SUCCESSFUL</t>
+  </si>
+  <si>
+    <t>Feature:</t>
+  </si>
+  <si>
+    <t>Registrar usuarios</t>
+  </si>
+  <si>
+    <t>Descripcion:</t>
+  </si>
+  <si>
+    <t>Yo como usuario de la plataforma</t>
+  </si>
+  <si>
+    <t>Quiero registrarme</t>
+  </si>
+  <si>
+    <t>Para poder loguearme en la plataforma</t>
+  </si>
+  <si>
+    <t>@RegistroIndefinido</t>
+  </si>
+  <si>
+    <t>Scenario:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given </t>
+  </si>
+  <si>
+    <t>que un usuario desea registrarse en la plataforma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When </t>
+  </si>
+  <si>
+    <t>ingresa datos de registros no definidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Then </t>
+  </si>
+  <si>
+    <t>debera vizualizar un mensaje de error "Solo los usuarios definidos logran el registro"</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>@RegistroSinContraseña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario: </t>
+  </si>
+  <si>
+    <t>Given</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> que un usuario desea registrarse en la plataforma</t>
+  </si>
+  <si>
+    <t>no ingresa un password</t>
+  </si>
+  <si>
+    <t>debera recibir un mensaje de error "password faltante"</t>
+  </si>
+  <si>
+    <t>@RegistroSinEmail</t>
+  </si>
+  <si>
+    <t>no ingresa un email</t>
+  </si>
+  <si>
+    <t>debera recibir un mensaje de error "email faltante"</t>
+  </si>
+  <si>
+    <t>@RegistroExitoso</t>
+  </si>
+  <si>
+    <t>ingresa datos de registros definidos</t>
+  </si>
+  <si>
+    <t>Recibira un id y un token de registro</t>
+  </si>
+  <si>
+    <t>Registro de usuarios</t>
+  </si>
+  <si>
+    <t>Yo como usuario de la pagina web de la tienda cereza</t>
+  </si>
+  <si>
+    <t>Para poder loguearme en la pagina web</t>
+  </si>
+  <si>
+    <t>@CamposObligatorios</t>
+  </si>
+  <si>
+    <t>que esta en la seccion de registro de la pagina web de la tienda cereza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intenta relizar un registro sin llenar los campos obligatorios </t>
+  </si>
+  <si>
+    <t>debera recibir un mensaje de error "Los campos de email y password son obligatorios"</t>
+  </si>
+  <si>
+    <t>@CamposNoObligatorios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intenta relizar un registro sin llenar los no campos obligatorios </t>
+  </si>
+  <si>
+    <t>debera  recibir un correo para confirmar el registro a la tienda</t>
+  </si>
+  <si>
+    <t>@UsarioYaRegistrado</t>
+  </si>
+  <si>
+    <t>intenta realizar el registro con un email ya registrado</t>
+  </si>
+  <si>
+    <t>debera recibir un mensaje de error "Esta dirección de e‑mail ya ha sido asociada con una cuenta"</t>
+  </si>
+  <si>
+    <t>@PasswordMinimo</t>
+  </si>
+  <si>
+    <t>intenta realizar el registro con un password de menos de 5 caracteres</t>
+  </si>
+  <si>
+    <t>debera recibir un mensaje de error "El password debe contener minimo 5 caracteres"</t>
+  </si>
+  <si>
+    <t>Inicio de Sesión</t>
+  </si>
+  <si>
+    <t>Yo como usuario registrado de la pagina web de la tienda cereza</t>
+  </si>
+  <si>
+    <t>Quiero poder inciar sesión</t>
+  </si>
+  <si>
+    <t>Para poder realizar la compra de productos</t>
+  </si>
+  <si>
+    <t>@PasswordVacio</t>
+  </si>
+  <si>
+    <t>que esta en la seccion de inicio de sesion de la pagina web de la tienda cereza</t>
+  </si>
+  <si>
+    <t>intenta iniciar sesión sin contraseña</t>
+  </si>
+  <si>
+    <t>debera recibir un mensaje de error "password requerido"</t>
+  </si>
+  <si>
+    <t>@EmailVacio</t>
+  </si>
+  <si>
+    <t>intenta iniciar sesión sin email</t>
+  </si>
+  <si>
+    <t>debera recibir un mensaje de error "email requerido"</t>
+  </si>
+  <si>
+    <t>@LoginExitoso</t>
+  </si>
+  <si>
+    <t>ingresa credenciales validas</t>
+  </si>
+  <si>
+    <t>debera redireccionarse al home page</t>
+  </si>
+  <si>
+    <t>@UsuarioNoRegistrado</t>
+  </si>
+  <si>
+    <t>ingresa credenciales no registradas</t>
+  </si>
+  <si>
+    <t>debera recibir un mensaje de error "el usuario no existe"</t>
+  </si>
+  <si>
+    <t>@PasswordIncorrecto</t>
+  </si>
+  <si>
+    <t>ingresa un password incorrecto</t>
+  </si>
+  <si>
+    <t>debera recibir un mensaje de error "contraseña incorrecta"</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -534,143 +863,82 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
+5. Verificar la visualización de un mensaje de bienvenida y la redirección a la homepage.
 </t>
     </r>
   </si>
   <si>
-    <t>Se recomienda ejecutar pruebas de seguridad.
-Se recomienda ejecutar pruebas de rendimiento.
-Se recomienda ejecutar pruebas de estrés.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se probará que se exijan campos mínimos para el registro.
-Se realizaran registros con diferentes combinaciones de correo y contraseña, ya sean existentes o no, con longitudes de contraseña variantes.
-</t>
-  </si>
-  <si>
-    <t>Se probará el ingreso de usuarios que se hayan creado y usuarios que no se sepa de su existencia en la BD de la página.
-Se realizarán ingresos de usuario con los campos vacíos de correo o contraseña.</t>
-  </si>
-  <si>
-    <t>CP01</t>
-  </si>
-  <si>
-    <t>CP02</t>
-  </si>
-  <si>
-    <t>CP03</t>
-  </si>
-  <si>
-    <t>CP04</t>
-  </si>
-  <si>
-    <t>Número de página a consultar como parametro</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">No hace parte del alcance:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>No es objeto de prueba la verificación de funcionalidades que no hagan parte del sistema de registro en la Tienda Cereza 🍒.
-Tampoco se tendrá en cuenta pruebas de seguridad, rendimiento y estrés.</t>
-    </r>
-  </si>
-  <si>
-    <t>Se recibió una respuesta con el STATUS: 200 OK.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Recibir una respuesta en formato JSON, así:
-{
-    "page": 2,
-    "per_page": 6,
-    "total": 1,
-    "total_pages": 2,
-    "data": [
-        {
-            "id": 7,
-            "email": "nombre.last@reqres.in",
-            "first_name": "Nombre",
-            "last_name": "Last",
-            "avatar": "image.jpg"
-        },
-    ],
-    "support": {
-        "url": "https://reqres.in/#support-heading",
-        "text": "Help!"
-    }
-}
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Se recibió una respuesta en formato JSON, así:
-{
-    "page": 2,
-    "per_page": 6,
-    "total": 1,
-    "total_pages": 2,
-    "data": [
-        {
-            "id": 7,
-            "email": "nombre.last@reqres.in",
-            "first_name": "Nombre",
-            "last_name": "Last",
-            "avatar": "image.jpg"
-        },
-    ],
-    "support": {
-        "url": "https://reqres.in/#support-heading",
-        "text": "Help!"
-    }
-}
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Se recibió una respuesta en formato JSON, así:
-{
-    "page": 1,
-    "per_page": 6,
-    "total": 1,
-    "total_pages": 2,
-    "data": [
-        {
-            "id": 7,
-            "email": "nombre.last@reqres.in",
-            "first_name": "Nombre",
-            "last_name": "Last",
-            "avatar": "image.jpg"
-        },
-    ],
-    "support": {
-        "url": "https://reqres.in/#support-heading",
-        "text": "Help!"
-    }
-}
-</t>
+    <t xml:space="preserve"> verificar que solo usuarios definidos puedan registrarse</t>
+  </si>
+  <si>
+    <t>verificar la vizualicion del mensaje de error cuando el campo email esta vacio</t>
+  </si>
+  <si>
+    <t>verificar que los usuarios definidos puedan registrarse</t>
+  </si>
+  <si>
+    <t>PÁGINA WEB TIENDA CEREZA</t>
+  </si>
+  <si>
+    <t>verificar el mensaje de error al ingresar un password incorrecto</t>
+  </si>
+  <si>
+    <t>verificar que se solicite de manera obligatoria los campos de correo y password en el formulario de registro</t>
+  </si>
+  <si>
+    <t>verificar que el usuario se pueda registrar sin llenar los campos de nombre y apellido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verificar que se puedan registrar solo usuarios que aun no estan registrados </t>
+  </si>
+  <si>
+    <t>verificar que el password ingresado contenga minimo 5 caracteres</t>
+  </si>
+  <si>
+    <t>verificar el mensaje de error al intentar iniciar sesión en la pagina sin password</t>
+  </si>
+  <si>
+    <t>verificar el mensaje de error al intentar iniciar sesión en la pagina sin email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verificar el ingreso satisfactorio a la tienda </t>
+  </si>
+  <si>
+    <t xml:space="preserve">verificar el mensaje de error al intentar ingresar con credenciales no registradas </t>
+  </si>
+  <si>
+    <t>Fallo del servicio.</t>
+  </si>
+  <si>
+    <t>Monitoreo constante de los servicios.</t>
+  </si>
+  <si>
+    <t>Interrupción en la red.</t>
+  </si>
+  <si>
+    <t>Proyecto</t>
+  </si>
+  <si>
+    <t>No se puede controlar la caída de la red.</t>
+  </si>
+  <si>
+    <t>Riesgos de servicios REQRES</t>
+  </si>
+  <si>
+    <t>Riesgos de Registro e Ingreso en Tienda Cereza 🍒</t>
+  </si>
+  <si>
+    <t>verificar la visualización del mensaje de error cuando el campo password esta vacío</t>
+  </si>
+  <si>
+    <t>Método Gherkin:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -715,13 +983,44 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -755,6 +1054,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
@@ -764,8 +1069,20 @@
         <bgColor rgb="FFD8D8D8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -855,11 +1172,127 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -876,7 +1309,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -885,7 +1318,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -895,16 +1328,16 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -917,6 +1350,67 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1248,8 +1742,8 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFF7E06"/>
       <color rgb="FFA5A5A5"/>
-      <color rgb="FFFF7E06"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1380,8 +1874,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>614469</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>812075</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>126275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1912,25 +2406,25 @@
         <v>19</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="162" x14ac:dyDescent="0.3">
@@ -1959,19 +2453,19 @@
         <v>23</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2099,31 +2593,31 @@
         <v>18</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="180" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="216" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -2140,28 +2634,28 @@
         <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>92</v>
+        <v>172</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="K5" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2178,8 +2672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480FDED1-1A1E-44D7-B872-85FF24D4C5DB}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2198,7 +2692,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="8"/>
+      <c r="A1" s="41" t="s">
+        <v>191</v>
+      </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -2207,7 +2703,7 @@
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="6"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="36" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -2217,62 +2713,62 @@
         <v>27</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:10" ht="36" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>186</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1">
         <f>E3*F3</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H3" s="1">
         <f>G3</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>57</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>58</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.3">
@@ -2280,10 +2776,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>59</v>
+        <v>188</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>56</v>
+        <v>189</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -2303,10 +2799,10 @@
         <v>5</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>61</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2314,10 +2810,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -2337,10 +2833,10 @@
         <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2348,10 +2844,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
@@ -2371,10 +2867,10 @@
         <v>25</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -2382,10 +2878,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -2405,10 +2901,10 @@
         <v>15</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -2416,10 +2912,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
@@ -2439,10 +2935,10 @@
         <v>5</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -2450,10 +2946,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -2473,10 +2969,10 @@
         <v>5</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -2484,10 +2980,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D10" s="3">
         <v>1</v>
@@ -2507,15 +3003,15 @@
         <v>10</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H10">
     <cfRule type="iconSet" priority="1">
@@ -2535,8 +3031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9E30F7-763E-44A1-AC72-B58C102A0249}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2555,16 +3051,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="6"/>
+      <c r="A1" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
     </row>
     <row r="2" spans="1:10" ht="36" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -2574,28 +3072,28 @@
         <v>27</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>51</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -2603,10 +3101,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -2626,10 +3124,10 @@
         <v>3</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -2637,10 +3135,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -2660,10 +3158,10 @@
         <v>5</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2671,10 +3169,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -2694,10 +3192,10 @@
         <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2705,10 +3203,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
@@ -2728,10 +3226,10 @@
         <v>25</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -2739,10 +3237,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -2762,10 +3260,10 @@
         <v>15</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -2773,10 +3271,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
@@ -2796,10 +3294,10 @@
         <v>5</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -2807,10 +3305,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -2830,10 +3328,10 @@
         <v>5</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -2841,10 +3339,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D10" s="3">
         <v>1</v>
@@ -2864,15 +3362,15 @@
         <v>10</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H10">
     <cfRule type="iconSet" priority="1">
@@ -2890,10 +3388,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF64FDF5-5E03-4C8A-948F-964343A0E4F3}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2920,149 +3418,164 @@
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:9" ht="36" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:9" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="24"/>
+    </row>
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B3" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D3" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F3" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I3" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="126" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="4" spans="1:9" ht="126" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="396" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="126" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="396" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="396" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="126" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="396" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3075,28 +3588,791 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2406D1D5-C0F8-4862-8277-1721ED58A928}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
+      <c r="B4" s="30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="27"/>
+      <c r="B5" s="30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="27"/>
+      <c r="B6" s="31"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="34"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="35"/>
+      <c r="B13" s="36"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="34"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="35"/>
+      <c r="B20" s="36"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="34"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="35"/>
+      <c r="B27" s="36"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="34"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A27:B27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FCE272-65CE-4E61-8DFF-1708BEA28DC8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
+      <c r="B4" s="39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="27"/>
+      <c r="B5" s="39" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="27"/>
+      <c r="B6" s="31"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="34"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="27"/>
+      <c r="B13" s="31"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="34"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="27"/>
+      <c r="B20" s="31"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="B21" s="34"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="27"/>
+      <c r="B27" s="31"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="34"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="27"/>
+      <c r="B36" s="30" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="27"/>
+      <c r="B37" s="30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="27"/>
+      <c r="B38" s="30"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" s="29"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" s="39" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" s="39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" s="39" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="39" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="27"/>
+      <c r="B45" s="31"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="B46" s="34"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B51" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="27"/>
+      <c r="B52" s="31"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="B53" s="34"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B54" s="39" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B55" s="39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B56" s="39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" s="39" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B58" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="27"/>
+      <c r="B59" s="31"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="B60" s="34"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B61" s="30" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B63" s="30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B64" s="30" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B65" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="27"/>
+      <c r="B66" s="31"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B67" s="34"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B68" s="39" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B69" s="39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B70" s="39" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B71" s="39" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B72" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
✨ Adding risks of both test plans
</commit_message>
<xml_diff>
--- a/PlanDePruebasRiesgosCasosDePrueba.xlsx
+++ b/PlanDePruebasRiesgosCasosDePrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\Training\Duras\Repos\C1-2023-QA-Calidad-T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31CEAFC-924F-40CA-87DB-FDE58C652999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C6AEB4-27E5-4346-8037-1B92ED12ADB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="5" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
   </bookViews>
   <sheets>
     <sheet name="PlaneDePruebaServicios" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="193">
   <si>
     <t>Célula</t>
   </si>
@@ -218,14 +218,6 @@
     <t>La pagina https://reqres.in debe estar en funcionamiento.</t>
   </si>
   <si>
-    <t>Estando dentro del entorno descrito en el apartado de contexto de la sección Alcance:
-1. Ingresar a la aplicación Postman.
-2. Crear una nueva HTTP Request de tipo GET.
-3. Ingresar la URL https://reqres.in/api/users?page=2 a esta petición.
-4. Enviarla.
-5. Revisar si la respuesta es la correcta.</t>
-  </si>
-  <si>
     <t>Recibir una respuesta con el STATUS: 200 OK.</t>
   </si>
   <si>
@@ -235,34 +227,9 @@
     <t>Verificar que el contenido de la respuesta corresponda al formato adecuado (JSON).</t>
   </si>
   <si>
-    <t>Estando dentro del entorno descrito en el apartado de contexto de la sección Alcance:
-1. Identificar los parámetros de la solicitud de la API.
-2. Ingresar a la aplicación Postman.
-3. Crear una nueva HTTP Request de tipo GET.
-4. Ingresar la URL https://reqres.in/api/users?page=2 a esta petición.
-5. Enviarla.
-6. Revisar que el cuerpo de la respuesta de la petición sea el correspondiente en el formato JSON.</t>
-  </si>
-  <si>
-    <t>Estando dentro del entorno descrito en el apartado de contexto de la sección Alcance:
-1. Ingresar a la aplicación Postman.
-2. Crear una nueva HTTP Request de tipo GET.
-3. Ingresar la URL https://reqres.in/api/users?page=2 a esta petición.
-4. Enviarla.
-5. Revisar si la respuesta a la petición es la correcta.</t>
-  </si>
-  <si>
     <t>Recibir respuesta a la petición con el body indicado.</t>
   </si>
   <si>
-    <t>Estando dentro del entorno descrito en el apartado de contexto de la sección Alcance:
-1. Ingresar a la aplicación Postman.
-2. Crear una nueva HTTP Request de tipo GET.
-3. Ingresar la URL https://reqres.in/api/users?page=%!"@#;¨^.
-4. Enviarla.
-5. Revisar si la respuesta a la petición es fallida.</t>
-  </si>
-  <si>
     <t>No pasó</t>
   </si>
   <si>
@@ -287,25 +254,13 @@
     <t>Plan de Acción</t>
   </si>
   <si>
-    <t>Mala determinación del tipo de respuesta HTTP.</t>
-  </si>
-  <si>
     <t>Producto</t>
   </si>
   <si>
     <t>Ignorar</t>
   </si>
   <si>
-    <t>Revisión y validación de la respuesta HTTP antes de permitir recibir peticiones.</t>
-  </si>
-  <si>
-    <t>Estructura JSON con formato erróneo.</t>
-  </si>
-  <si>
     <t>Mitigar</t>
-  </si>
-  <si>
-    <t>Reestructurar el JSON a ser entregado de la manera correcta.</t>
   </si>
   <si>
     <t>La petición no es aceptada a pesar de enviar un valor de parámetro correcto.</t>
@@ -932,6 +887,45 @@
   </si>
   <si>
     <t>Método Gherkin:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar a la aplicación Postman.
+2. Crear una nueva HTTP Request de tipo GET.
+3. Ingresar la URL https://reqres.in/api/users?page=2 a esta petición.
+4. Enviarla.
+5. Revisar si la respuesta es la correcta.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Identificar los parámetros de la solicitud de la API.
+2. Ingresar a la aplicación Postman.
+3. Crear una nueva HTTP Request de tipo GET.
+4. Ingresar la URL https://reqres.in/api/users?page=2 a esta petición.
+5. Enviarla.
+6. Revisar que el cuerpo de la respuesta de la petición sea el correspondiente en el formato JSON.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar a la aplicación Postman.
+2. Crear una nueva HTTP Request de tipo GET.
+3. Ingresar la URL https://reqres.in/api/users?page=2 a esta petición.
+4. Enviarla.
+5. Revisar si la respuesta a la petición es la correcta.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar a la aplicación Postman.
+2. Crear una nueva HTTP Request de tipo GET.
+3. Ingresar la URL https://reqres.in/api/users?page=%!"@#;¨^.
+4. Enviarla.
+5. Revisar si la respuesta a la petición es fallida.
+</t>
+  </si>
+  <si>
+    <t>Fallo del servicio de registro.</t>
+  </si>
+  <si>
+    <t>Fallo del servicio de ingreso.</t>
   </si>
 </sst>
 </file>
@@ -1866,16 +1860,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>473528</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>694508</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>27215</xdr:rowOff>
+      <xdr:rowOff>4355</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>614469</xdr:colOff>
+      <xdr:colOff>42969</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>126275</xdr:rowOff>
+      <xdr:rowOff>103415</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1905,8 +1899,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11522528" y="255815"/>
-          <a:ext cx="6498198" cy="3299460"/>
+          <a:off x="10935788" y="232955"/>
+          <a:ext cx="6480781" cy="3299460"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1940,8 +1934,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>692846</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>709749</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>115389</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2406,25 +2400,25 @@
         <v>19</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>22</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="162" x14ac:dyDescent="0.3">
@@ -2453,19 +2447,19 @@
         <v>23</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2593,28 +2587,28 @@
         <v>18</v>
       </c>
       <c r="F4" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="216" x14ac:dyDescent="0.3">
@@ -2634,28 +2628,28 @@
         <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2673,7 +2667,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2693,7 +2687,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -2713,28 +2707,28 @@
         <v>27</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>47</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="36" x14ac:dyDescent="0.3">
@@ -2742,10 +2736,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -2765,10 +2759,10 @@
         <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.3">
@@ -2776,10 +2770,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -2788,21 +2782,21 @@
         <v>1</v>
       </c>
       <c r="F4" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" ref="G4:G10" si="0">E4*F4</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" ref="H4:H10" si="1">G4</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2810,10 +2804,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -2833,10 +2827,10 @@
         <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2844,10 +2838,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
@@ -2867,10 +2861,10 @@
         <v>25</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -2878,10 +2872,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -2901,10 +2895,10 @@
         <v>15</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -2912,33 +2906,33 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
       </c>
       <c r="E8" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8" s="4">
         <v>5</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -2946,33 +2940,33 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9" s="2">
         <v>5</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="54" x14ac:dyDescent="0.3">
@@ -2980,10 +2974,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D10" s="3">
         <v>1</v>
@@ -3003,10 +2997,10 @@
         <v>10</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3031,8 +3025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9E30F7-763E-44A1-AC72-B58C102A0249}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3052,7 +3046,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B1" s="41"/>
       <c r="C1" s="41"/>
@@ -3072,307 +3066,197 @@
         <v>27</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:10" ht="36" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>191</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1">
         <f>E3*F3</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H3" s="1">
         <f>G3</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>192</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
       </c>
       <c r="E4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="4">
         <v>5</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" ref="G4:G10" si="0">E4*F4</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" ref="H4:H10" si="1">G4</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2">
         <v>5</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>E5*F5</f>
+        <v>15</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <f>G5</f>
+        <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4">
-        <v>5</v>
-      </c>
-      <c r="F6" s="3">
-        <v>5</v>
-      </c>
-      <c r="G6" s="4">
-        <f>E6*F6</f>
-        <v>25</v>
-      </c>
-      <c r="H6" s="3">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="54" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <v>3</v>
-      </c>
-      <c r="F7" s="2">
-        <v>5</v>
-      </c>
-      <c r="G7" s="1">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="H7" s="1">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="54" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3">
-        <v>5</v>
-      </c>
-      <c r="G8" s="4">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H8" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="54" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
-        <v>5</v>
-      </c>
-      <c r="G9" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H9" s="1">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="54" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4">
-        <v>5</v>
-      </c>
-      <c r="F10" s="3">
-        <v>2</v>
-      </c>
-      <c r="G10" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H10" s="3">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>71</v>
-      </c>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="H3:H10">
+  <conditionalFormatting sqref="H3:H5">
     <cfRule type="iconSet" priority="1">
       <iconSet showValue="0" reverse="1">
         <cfvo type="percent" val="0"/>
@@ -3391,7 +3275,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3421,10 +3305,10 @@
     <row r="2" spans="1:9" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="21" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -3462,12 +3346,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="126" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="108" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>34</v>
@@ -3476,19 +3360,19 @@
         <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="396" x14ac:dyDescent="0.3">
@@ -3496,57 +3380,57 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>40</v>
+        <v>188</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="126" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="108" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>41</v>
+        <v>189</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="396" x14ac:dyDescent="0.3">
@@ -3554,28 +3438,28 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>43</v>
+        <v>190</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3590,7 +3474,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2406D1D5-C0F8-4862-8277-1721ED58A928}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3600,38 +3486,38 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="27"/>
       <c r="B4" s="30" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="27"/>
       <c r="B5" s="30" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3640,48 +3526,48 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B7" s="34"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3690,48 +3576,48 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="33" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B14" s="34"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="30" t="s">
         <v>121</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3740,48 +3626,48 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="33" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B21" s="34"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3790,48 +3676,48 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="33" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B28" s="34"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="26" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -3860,38 +3746,38 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="27"/>
       <c r="B4" s="39" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="27"/>
       <c r="B5" s="39" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3900,48 +3786,48 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B7" s="34"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3950,48 +3836,48 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="33" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B14" s="34"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4000,48 +3886,48 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="33" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B21" s="34"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4050,76 +3936,76 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="33" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B28" s="34"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="26" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="25" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="26" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="27"/>
       <c r="B36" s="30" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="27"/>
       <c r="B37" s="30" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4128,48 +4014,48 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="33" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B39" s="29"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="26" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="26" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="26" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4178,48 +4064,48 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="33" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B46" s="34"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="26" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="26" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="26" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4228,48 +4114,48 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="33" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B53" s="34"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="26" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="26" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="26" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B58" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4278,48 +4164,48 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="33" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B60" s="34"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="26" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B61" s="30" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="26" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="26" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4328,48 +4214,48 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="33" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B67" s="34"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="26" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="26" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="26" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B70" s="39" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B72" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
✨ Adding additional risks in both test plans
</commit_message>
<xml_diff>
--- a/PlanDePruebasRiesgosCasosDePrueba.xlsx
+++ b/PlanDePruebasRiesgosCasosDePrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\Training\Duras\Repos\C1-2023-QA-Calidad-T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C6AEB4-27E5-4346-8037-1B92ED12ADB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E71A799-86E6-4067-9B7D-286CF761291C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
   </bookViews>
   <sheets>
     <sheet name="PlaneDePruebaServicios" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="203">
   <si>
     <t>Célula</t>
   </si>
@@ -926,6 +926,36 @@
   </si>
   <si>
     <t>Fallo del servicio de ingreso.</t>
+  </si>
+  <si>
+    <t>Realizar cambio de función del botón en front-end.</t>
+  </si>
+  <si>
+    <t>El botón de ingreso no funciona.</t>
+  </si>
+  <si>
+    <t>Falta de recursos para el host de la página.</t>
+  </si>
+  <si>
+    <t>Se transfiere la responsabilidad al PO debido a que es un tema económico.</t>
+  </si>
+  <si>
+    <t>Los mensajes de error contienen caracteres ilegibles</t>
+  </si>
+  <si>
+    <t>Monitorear la ortografía de los recursos a mostrar en el front-end.</t>
+  </si>
+  <si>
+    <t>Las URL no direccionan donde deberían.</t>
+  </si>
+  <si>
+    <t>Es una característica de la que se encarga el proveedor del host.</t>
+  </si>
+  <si>
+    <t>El botón de crear usuario se bloquea al darle un primer clic.</t>
+  </si>
+  <si>
+    <t>Realizar un control en la función del botón con respecto a la conexión con la BD de usuarios.</t>
   </si>
 </sst>
 </file>
@@ -1934,8 +1964,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>692846</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>115389</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>252549</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2287,7 +2317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EA6F44-0A13-4B3B-95DA-2DE7B9084CBB}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
@@ -2666,8 +2696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480FDED1-1A1E-44D7-B872-85FF24D4C5DB}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3023,16 +3053,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9E30F7-763E-44A1-AC72-B58C102A0249}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.21875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" style="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5546875" style="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" style="20"/>
     <col min="5" max="5" width="16" style="20" bestFit="1" customWidth="1"/>
@@ -3148,7 +3178,7 @@
         <v>10</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ref="H4:H10" si="1">G4</f>
+        <f t="shared" ref="H4:H13" si="1">G4</f>
         <v>10</v>
       </c>
       <c r="I4" s="3" t="s">
@@ -3186,77 +3216,223 @@
         <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
+    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" ref="G6:G13" si="2">E6*F6</f>
+        <v>3</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>4</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="H3:H5">
+  <conditionalFormatting sqref="H3:H10">
     <cfRule type="iconSet" priority="1">
       <iconSet showValue="0" reverse="1">
         <cfvo type="percent" val="0"/>
@@ -3275,7 +3451,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3474,9 +3650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2406D1D5-C0F8-4862-8277-1721ED58A928}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3734,9 +3908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FCE272-65CE-4E61-8DFF-1708BEA28DC8}">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
✨ Adding defect reports for services
</commit_message>
<xml_diff>
--- a/PlanDePruebasRiesgosCasosDePrueba.xlsx
+++ b/PlanDePruebasRiesgosCasosDePrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\Training\Duras\Repos\C1-2023-QA-Calidad-T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E71A799-86E6-4067-9B7D-286CF761291C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF8581C-0290-4BB0-92EA-7D20BF1C3610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="5" activeTab="7" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
   </bookViews>
   <sheets>
     <sheet name="PlaneDePruebaServicios" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="CPServicioGET" sheetId="3" r:id="rId5"/>
     <sheet name="CPServicioPOST" sheetId="4" r:id="rId6"/>
     <sheet name="CPLoginRegistroTiendaCereza" sheetId="5" r:id="rId7"/>
+    <sheet name="GestiónDeDefectosSerivios" sheetId="9" r:id="rId8"/>
+    <sheet name="GestiónDeDefectosTiendaCereza" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="247">
   <si>
     <t>Célula</t>
   </si>
@@ -957,12 +959,848 @@
   <si>
     <t>Realizar un control en la función del botón con respecto a la conexión con la BD de usuarios.</t>
   </si>
+  <si>
+    <t>@MensajeConfirmación</t>
+  </si>
+  <si>
+    <t>verificar la visualización del mensaje informando envío de correo de confirmación</t>
+  </si>
+  <si>
+    <t>se registra con los campos obligatorios</t>
+  </si>
+  <si>
+    <t>debera  recibir un mensaje informando el envío de un correo de confirmación del registro a la tienda</t>
+  </si>
+  <si>
+    <t>ingresa un password incorrecto más de 5 veces</t>
+  </si>
+  <si>
+    <t>@LímiteIngresosFallidos</t>
+  </si>
+  <si>
+    <t>verificar que exista un límite de 5 intentos fallidos al ingresar un password incorrecto</t>
+  </si>
+  <si>
+    <t>debera recibir un mensaje de error informando el bloqueo temporal de la cuenta</t>
+  </si>
+  <si>
+    <t>verificar que el password no contenga información personal</t>
+  </si>
+  <si>
+    <t>intenta realizar un registro con una contraseña que contiene información personal</t>
+  </si>
+  <si>
+    <t>debera recibir un mensaje de error "Contraseña débil o insegura, no use información personal"</t>
+  </si>
+  <si>
+    <t>@PasswordInseguro</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> BUG1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fecha:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 28/02/2023</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Título:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> No se muestra el mensaje de error al enviar el parámetro de página incorrecto</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resumen:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Se envia una petición con un parámetro de página, por ejemplo page=%!"@#;¨^ y el servicio me retorna el contenido de la página 1 (es decir, como si page=1) en lugar de retornar un error.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Autor:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Miguel Molina</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Versión:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> V1.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ambiente:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Postman</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fase:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Operación</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Para lograr reproducir este bug, es necesario seguir los pasos siguientes:
+1. Ingresar a la aplicación Postman.
+2. Crear una nueva HTTP Request de tipo GET.
+3. Ingresar la URL https://reqres.in/api/users?page=%!"@#;¨^.
+4. Enviarla.
+5. Visualizar la respuesta inadecuada, es decir el bug.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Estado: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Por hacer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prioridad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alcance/Impacto:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nota: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>la escala de prioridad va de 1 a 5, donde 1 es prioridad mínima y 5 es máxima. Y la escala de impacto es igual a la presentada en los riesgos (1 despreciable - 5 catastrofico).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resultados esperados:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Mensaje de error informando que el parámetro page ingresado es invalido.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resultados Obtenidos:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Contenido JSON del parámetro page=1.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Historial:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Miguel Molina -&gt; (Por hacer)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Áreas afectadas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Interfaz de usuario.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Referencias:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Este bug se deriva del CP04</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Informe de Defectos Servicios</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> BUG2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Título:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> No se muestra el mensaje de error al ingresar una contraseña con menos de 5 caracteres</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Autor:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Jonathan Vargas</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alcance/Impacto:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Historial:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Jonathan Vargas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -&gt; (Por hacer)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Referencias:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Este bug se deriva del CP @PasswordMinimo</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Para lograr reproducir este bug, es necesario seguir los pasos siguientes:
+1. Ingresar a la aplicación Postman.
+2. Crear una nueva HTTP Request de tipo POST.
+3. Ingresar la URL https://reqres.in/api/register.
+4. Ingresar un cuerpo con el siguiente formato:
+  {
+    "email": "eve.holt@reqres.in",
+    "password": "pass"
+  }
+5. Enviar la petición.
+6. Visualizar el código de respuesta OK y token de registro.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resultados Obtenidos:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Código de respuesta 200 OK y JSON con token de registro.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resultados esperados:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Mensaje de error informando que el campo de password debe contener mínimo 5 caracteres.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Áreas afectadas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Base de datos y área de seguridad.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nota: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>la escala de prioridad va de 1 a 5, donde 1 es prioridad mínima y 5 es máxima. Y la escala de impacto es igual a la presentada en los riesgos (1 despreciable - 5 catastrófico).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resumen:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Se envía una petición GET con un parámetro de página, por ejemplo page=%!"@#;¨^ y el servicio me retorna el contenido de la página 1 (es decir, como si page=1) en lugar de retornar un error.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resumen:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Se envía una petición POST con cuerpo donde el campo de password contiene menos de 5 caracteres, y el servicio me recibe el registro satisfactoriamente y no muestra un mensaje de error.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1043,8 +1881,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1105,8 +1960,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1312,11 +2173,219 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF7E06"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF7E06"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF7E06"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF7E06"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF7E06"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF7E06"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF7E06"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF7E06"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF7E06"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF7E06"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF7E06"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF7E06"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF7E06"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF7E06"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF7E06"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF7E06"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF7E06"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF7E06"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF7E06"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF7E06"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF7E06"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF7E06"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF7E06"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF7E06"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF7E06"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF7E06"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1339,9 +2408,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1358,12 +2424,6 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1416,26 +2476,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2315,9 +3487,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EA6F44-0A13-4B3B-95DA-2DE7B9084CBB}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
@@ -2340,114 +3515,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
     </row>
     <row r="2" spans="1:13" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-    </row>
-    <row r="3" spans="1:13" s="10" customFormat="1" ht="36" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+    </row>
+    <row r="3" spans="1:13" s="9" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="180" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="10" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2506,10 +3681,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52918882-42F7-4A79-8BF7-71EFDDF0321F}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2530,114 +3708,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
     </row>
     <row r="2" spans="1:13" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-    </row>
-    <row r="3" spans="1:13" s="9" customFormat="1" ht="36" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+    </row>
+    <row r="3" spans="1:13" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="162" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="10" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2694,70 +3872,73 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480FDED1-1A1E-44D7-B872-85FF24D4C5DB}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="20"/>
-    <col min="5" max="5" width="16" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="20"/>
-    <col min="8" max="8" width="10.5546875" style="20" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38" style="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.5546875" style="20"/>
+    <col min="1" max="1" width="3.5546875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="17"/>
+    <col min="5" max="5" width="16" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="17"/>
+    <col min="8" max="8" width="10.5546875" style="17" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.5546875" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
     </row>
     <row r="2" spans="1:10" ht="36" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="14" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2815,7 +3996,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" ref="G4:G10" si="0">E4*F4</f>
+        <f t="shared" ref="G4:G9" si="0">E4*F4</f>
         <v>2</v>
       </c>
       <c r="H4" s="3">
@@ -3053,70 +4234,73 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9E30F7-763E-44A1-AC72-B58C102A0249}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="A2" sqref="A2:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="20"/>
-    <col min="5" max="5" width="16" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="20"/>
-    <col min="8" max="8" width="10.5546875" style="20" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.21875" style="20" customWidth="1"/>
-    <col min="11" max="16384" width="11.5546875" style="20"/>
+    <col min="1" max="1" width="3.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="17"/>
+    <col min="5" max="5" width="16" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="17"/>
+    <col min="8" max="8" width="10.5546875" style="17" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.21875" style="17" customWidth="1"/>
+    <col min="11" max="16384" width="11.5546875" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" ht="36" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="14" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3174,11 +4358,11 @@
         <v>5</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" ref="G4:G10" si="0">E4*F4</f>
+        <f t="shared" ref="G4" si="0">E4*F4</f>
         <v>10</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ref="H4:H13" si="1">G4</f>
+        <f t="shared" ref="H4:H10" si="1">G4</f>
         <v>10</v>
       </c>
       <c r="I4" s="3" t="s">
@@ -3242,7 +4426,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" ref="G6:G13" si="2">E6*F6</f>
+        <f t="shared" ref="G6:G10" si="2">E6*F6</f>
         <v>3</v>
       </c>
       <c r="H6" s="3">
@@ -3280,7 +4464,7 @@
         <v>20</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="1"/>
+        <f>G7</f>
         <v>20</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -3448,10 +4632,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF64FDF5-5E03-4C8A-948F-964343A0E4F3}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3468,22 +4655,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="39"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+    </row>
+    <row r="2" spans="1:9" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>95</v>
       </c>
       <c r="D2" s="6"/>
@@ -3491,34 +4678,34 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="24"/>
+      <c r="I2" s="21"/>
     </row>
     <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="15" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3648,9 +4835,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2406D1D5-C0F8-4862-8277-1721ED58A928}">
-  <dimension ref="A1:B33"/>
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3659,239 +4851,289 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="33" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="27" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="27"/>
-      <c r="B4" s="30" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="27" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
-      <c r="B5" s="30" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="27" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="27"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="28"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="34"/>
+      <c r="B7" s="31"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="27" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="27" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="27" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="27" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="35"/>
-      <c r="B13" s="36"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="41"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="B14" s="34"/>
+      <c r="B14" s="31"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="27" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="27" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="27" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="27" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="41"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="34"/>
+      <c r="B21" s="31"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="27" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="27" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="27" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="27" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="35"/>
-      <c r="B27" s="36"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="41"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="34"/>
+      <c r="B28" s="31"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="27" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="27" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="27" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="27" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="29" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="43"/>
+      <c r="B34" s="44"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" s="31"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="42" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3901,536 +5143,1048 @@
     <mergeCell ref="A27:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FCE272-65CE-4E61-8DFF-1708BEA28DC8}">
-  <dimension ref="A1:B72"/>
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="89.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="35" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="34" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="27"/>
-      <c r="B4" s="39" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="34" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
-      <c r="B5" s="39" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="34" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="27"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="28"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="34"/>
+      <c r="B7" s="31"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="34" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="34" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="34" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="34" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="27"/>
-      <c r="B13" s="31"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="46"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" s="31"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="24"/>
+      <c r="B20" s="28"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="B14" s="34"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+      <c r="B21" s="31"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B22" s="34" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B23" s="34" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B24" s="34" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B25" s="27" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="28" t="s">
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B26" s="29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="27"/>
-      <c r="B20" s="31"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="33" t="s">
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="24"/>
+      <c r="B27" s="28"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="B21" s="34"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
+      <c r="B28" s="31"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B29" s="34" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="26" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B30" s="34" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="26" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B31" s="34" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="26" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B32" s="34" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="28" t="s">
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B33" s="29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="27"/>
-      <c r="B27" s="31"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="33" t="s">
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="45"/>
+      <c r="B34" s="46"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="B35" s="31"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="34" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="47"/>
+      <c r="B41" s="48"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="34"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="26" t="s">
+      <c r="B42" s="31"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B43" s="27" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B44" s="27" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="26" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B45" s="27" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="26" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B46" s="27" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="28" t="s">
+    <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B47" s="29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="25" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B48" s="26" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="26" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B49" s="27" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="27"/>
-      <c r="B36" s="30" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="24"/>
+      <c r="B50" s="27" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="27"/>
-      <c r="B37" s="30" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="24"/>
+      <c r="B51" s="27" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="27"/>
-      <c r="B38" s="30"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="33" t="s">
+    <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="24"/>
+      <c r="B52" s="27"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="B39" s="29"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="26" t="s">
+      <c r="B53" s="26"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B40" s="39" t="s">
+      <c r="B54" s="34" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="26" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B41" s="39" t="s">
+      <c r="B55" s="34" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="26" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B42" s="39" t="s">
+      <c r="B56" s="34" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="26" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B43" s="39" t="s">
+      <c r="B57" s="34" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="28" t="s">
+    <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="B58" s="29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="27"/>
-      <c r="B45" s="31"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="33" t="s">
+    <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="24"/>
+      <c r="B59" s="28"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="B46" s="34"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="26" t="s">
+      <c r="B60" s="31"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B61" s="27" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="26" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B48" s="30" t="s">
+      <c r="B62" s="27" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="26" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="30" t="s">
+      <c r="B63" s="27" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="26" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B50" s="30" t="s">
+      <c r="B64" s="27" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="28" t="s">
+    <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B51" s="32" t="s">
+      <c r="B65" s="29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="27"/>
-      <c r="B52" s="31"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="33" t="s">
+    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="24"/>
+      <c r="B66" s="28"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="B53" s="34"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="26" t="s">
+      <c r="B67" s="31"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="39" t="s">
+      <c r="B68" s="34" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="26" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B55" s="39" t="s">
+      <c r="B69" s="34" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="26" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B56" s="39" t="s">
+      <c r="B70" s="34" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="26" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B57" s="39" t="s">
+      <c r="B71" s="34" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="28" t="s">
+    <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B58" s="32" t="s">
+      <c r="B72" s="29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="27"/>
-      <c r="B59" s="31"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="33" t="s">
+    <row r="73" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="24"/>
+      <c r="B73" s="28"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="B60" s="34"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="26" t="s">
+      <c r="B74" s="31"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B61" s="30" t="s">
+      <c r="B75" s="27" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="26" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B62" s="30" t="s">
+      <c r="B76" s="27" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="26" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B63" s="30" t="s">
+      <c r="B77" s="27" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="26" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B64" s="30" t="s">
+      <c r="B78" s="27" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="28" t="s">
+    <row r="79" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B65" s="32" t="s">
+      <c r="B79" s="29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="27"/>
-      <c r="B66" s="31"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="33" t="s">
+    <row r="80" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="24"/>
+      <c r="B80" s="28"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="B67" s="34"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="26" t="s">
+      <c r="B81" s="31"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B68" s="39" t="s">
+      <c r="B82" s="34" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="26" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B69" s="39" t="s">
+      <c r="B83" s="34" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="26" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B70" s="39" t="s">
+      <c r="B84" s="34" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="26" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B71" s="39" t="s">
+      <c r="B85" s="34" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="28" t="s">
+    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B72" s="32" t="s">
+      <c r="B86" s="29" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="47"/>
+      <c r="B87" s="48"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="B88" s="31"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B89" s="34" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B90" s="34" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B91" s="34" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B92" s="34" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B93" s="42" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0993C8F5-BDF9-42D6-873D-DAC0BD643BE2}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="5"/>
+    <col min="5" max="5" width="61.6640625" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="11.5546875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="74" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="73"/>
+    </row>
+    <row r="2" spans="1:5" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="68" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="70"/>
+      <c r="E2" s="49" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5" s="53"/>
+    </row>
+    <row r="6" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B6" s="54"/>
+      <c r="C6" s="55"/>
+    </row>
+    <row r="7" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B7" s="56"/>
+      <c r="C7" s="57"/>
+    </row>
+    <row r="8" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8" s="58" t="s">
+        <v>229</v>
+      </c>
+      <c r="C8" s="59"/>
+    </row>
+    <row r="9" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="63" t="s">
+        <v>231</v>
+      </c>
+      <c r="B9" s="64"/>
+      <c r="C9" s="65"/>
+    </row>
+    <row r="10" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="58" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10" s="66"/>
+      <c r="C10" s="59"/>
+    </row>
+    <row r="11" spans="1:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="54" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="67"/>
+      <c r="C11" s="55"/>
+    </row>
+    <row r="12" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="71"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="73"/>
+    </row>
+    <row r="13" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="75" t="s">
+        <v>234</v>
+      </c>
+      <c r="B13" s="76" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="70"/>
+    </row>
+    <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B16" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="C16" s="53"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B17" s="54"/>
+      <c r="C17" s="55"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B18" s="56"/>
+      <c r="C18" s="57"/>
+    </row>
+    <row r="19" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B19" s="78" t="s">
+        <v>241</v>
+      </c>
+      <c r="C19" s="59"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="63" t="s">
+        <v>243</v>
+      </c>
+      <c r="B20" s="64"/>
+      <c r="C20" s="65"/>
+    </row>
+    <row r="21" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="60" t="s">
+        <v>238</v>
+      </c>
+      <c r="B21" s="61"/>
+      <c r="C21" s="62"/>
+    </row>
+    <row r="22" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="63" t="s">
+        <v>239</v>
+      </c>
+      <c r="B22" s="64"/>
+      <c r="C22" s="65"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B16:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B5:C7"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="B8:C8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67ACC392-DCEC-48D7-82D4-3A162F98740F}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="5"/>
+    <col min="5" max="5" width="61.6640625" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="11.5546875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+    </row>
+    <row r="2" spans="1:5" s="5" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="51"/>
+      <c r="E2" s="49" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5" s="53"/>
+    </row>
+    <row r="6" spans="1:5" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B6" s="54"/>
+      <c r="C6" s="55"/>
+    </row>
+    <row r="7" spans="1:5" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B7" s="56"/>
+      <c r="C7" s="57"/>
+    </row>
+    <row r="8" spans="1:5" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8" s="58" t="s">
+        <v>229</v>
+      </c>
+      <c r="C8" s="59"/>
+    </row>
+    <row r="9" spans="1:5" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="63" t="s">
+        <v>231</v>
+      </c>
+      <c r="B9" s="64"/>
+      <c r="C9" s="65"/>
+    </row>
+    <row r="10" spans="1:5" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="60" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10" s="61"/>
+      <c r="C10" s="62"/>
+    </row>
+    <row r="11" spans="1:5" s="5" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="63" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="64"/>
+      <c r="C11" s="65"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B5:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
✨ Adding defect reports for Tienda Cereza
</commit_message>
<xml_diff>
--- a/PlanDePruebasRiesgosCasosDePrueba.xlsx
+++ b/PlanDePruebasRiesgosCasosDePrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\Training\Duras\Repos\C1-2023-QA-Calidad-T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF8581C-0290-4BB0-92EA-7D20BF1C3610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4214BD39-8C5A-416C-8310-6B5B21C905FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="5" activeTab="7" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
   </bookViews>
   <sheets>
     <sheet name="PlaneDePruebaServicios" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="272">
   <si>
     <t>Célula</t>
   </si>
@@ -1074,30 +1074,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Resumen:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Se envia una petición con un parámetro de página, por ejemplo page=%!"@#;¨^ y el servicio me retorna el contenido de la página 1 (es decir, como si page=1) en lugar de retornar un error.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Autor:</t>
     </r>
     <r>
@@ -1381,28 +1357,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Miguel Molina -&gt; (Por hacer)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Áreas afectadas:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Interfaz de usuario.</t>
     </r>
   </si>
   <si>
@@ -1704,28 +1658,6 @@
     <r>
       <rPr>
         <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Áreas afectadas:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Base de datos y área de seguridad.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
         <i/>
         <sz val="10"/>
         <color theme="1"/>
@@ -1793,6 +1725,735 @@
       </rPr>
       <t xml:space="preserve">
 Se envía una petición POST con cuerpo donde el campo de password contiene menos de 5 caracteres, y el servicio me recibe el registro satisfactoriamente y no muestra un mensaje de error.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Referencias:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Este bug se deriva del CP @MensajeConfirmación</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Referencias:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Este bug se deriva del CP @PasswordInseguro</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Referencias:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Este bug se deriva del CP @LímiteIngresosFallidos</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> BUG3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> BUG4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> BUG5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Título:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> No se muestra el mensaje de información del envío de un correo de confirmación de registro. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resumen:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Se registra un usuario de manera satisfactoria, y se redireciona directamente a la página del perfil del usuario, sin antes mostrar el mensaje informando el enivio del correo de confirmación.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ambiente:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Navegador Opera GX.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prioridad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Para lograr reproducir este bug, es necesario seguir los pasos siguientes:
+1. Abrir el navegador Opera GX.
+2. Ingresar la URL https://tiendacereza.com/account/register.
+3. Identificar los campos obligatorios de correo y contraseña.
+4. Digitar valores validos para los campos obligatorios.
+5. Identificar el botón Crear.
+6. Dar clic en el botón Crear.
+7. Redireccionamiento al perfil del usuario registrado sin mensaje de información de envio de correo.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resultados Obtenidos:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Redireccionamiento a la página de perfil de usuario.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resultados esperados:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Redireccionamiento a la página de ingreso, visualización de un mensaje de información sobre el envío de correo de confirmación.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Título:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Se permite el registro de un usuario con una contraseña que contiene información personal</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resumen:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Se registra un usuario de manera satisfactoria con una contraseña que contiene información personal, y se acepta el registro cono válido, en lugar de impedirlo y mostrar un mensaje de error informando que la contraseña es débil o insegura.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Para lograr reproducir este bug, es necesario seguir los pasos siguientes:
+1. Abrir el navegador Opera GX.
+2. Ingresar la URL https://tiendacereza.com/account/register.
+3. Identificar los campos obligatorios de correo y contraseña y no obligatorios de nombre y apellido.
+4. Digitar valores validos para los campos no obligatorios.
+5. Digitar valores validos para los campos obligatorios, donde la contraseña contiene al menos el valor de uno de los campos no obligatorios.
+6. Identificar el botón Crear.
+7. Dar clic en el botón Crear.
+8. Redireccionamiento al perfil del usuario registrado, en lugar de denegar el registro y mostrar el mensaje de error de contraseña débil o insegura.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resultados esperados:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Mensaje de error informando que la contraseña es débil o insegura.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resultados Obtenidos:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Registro exitoso y redireccionamiento a la página de perfil de usuario.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Áreas afectadas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> área de seguridad.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Áreas afectadas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> interfaz de usuario y área de seguridad.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Título:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Se permite ingresar más de 5 veces contraseñas incorrectas.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resumen:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Un usuario válido puede ingresar más de 5 veces contraseñas incorrectas, y no recibe una suspensión temporal de su cuenta.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Para lograr reproducir este bug, es necesario seguir los pasos siguientes:
+1. Abrir el navegador Opera GX.
+2. Ingresar la URL https://tiendacereza.com/account/login.
+3. Identificar los campos obligatorios de correo y contraseña.
+4. Digitar valores validos para el correo, pero no para la contraseña.
+5. Identificar el botón de Iniciar sesión.
+6. Dar clic en el botón de Iniciar sesión.
+7. Realizar los pasos 4, 5 y 6 nuevamente por lo menos 6 veces.
+8. No se evidencia un mensaje informando la suspensión temporal de la cuenta. Se permite realizar los pasos 4, 5 y 6 otra vez.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resultados Obtenidos:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Redirección a la página de ingreso con un mensaje de error de contraseña o correo invalidos. Se puede reingresar otra vez.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Resultados esperados:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Mensaje de error informando la suspension temporal de la cuenta, y se deniega el ingreso al mismo usuario nuevamente de manera temporal.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Áreas afectadas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> área de seguridad y vulnerabilidad.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Áreas afectadas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> interfaz de usuario.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Áreas afectadas:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> base de datos y área de seguridad.</t>
     </r>
   </si>
 </sst>
@@ -1967,7 +2628,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -2175,32 +2836,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFFF7E06"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFFF7E06"/>
       </left>
       <right/>
@@ -2336,6 +2971,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF7E06"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -2385,7 +3029,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2522,10 +3166,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2540,10 +3184,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2555,25 +3199,25 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2582,13 +3226,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2597,16 +3238,16 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3492,7 +4133,7 @@
   </sheetPr>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
@@ -3687,7 +4328,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3878,7 +4519,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4240,7 +4881,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J10"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4637,8 +5278,8 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4840,9 +5481,7 @@
   </sheetPr>
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5154,9 +5793,7 @@
   </sheetPr>
   <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5840,8 +6477,8 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -5855,22 +6492,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="74" t="s">
-        <v>233</v>
-      </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="73"/>
+      <c r="A1" s="73" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="72"/>
     </row>
     <row r="2" spans="1:5" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="67" t="s">
         <v>215</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="68" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="70"/>
+      <c r="C2" s="69"/>
       <c r="E2" s="49" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.3">
@@ -5878,164 +6515,164 @@
         <v>216</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B5" s="52" t="s">
-        <v>223</v>
-      </c>
-      <c r="C5" s="53"/>
+        <v>225</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" s="51"/>
     </row>
     <row r="6" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
+        <v>224</v>
+      </c>
+      <c r="B6" s="52"/>
+      <c r="C6" s="53"/>
     </row>
     <row r="7" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="57"/>
+        <v>223</v>
+      </c>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
     </row>
     <row r="8" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" s="56" t="s">
         <v>228</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="C8" s="57"/>
+    </row>
+    <row r="9" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="61" t="s">
+        <v>270</v>
+      </c>
+      <c r="B9" s="62"/>
+      <c r="C9" s="63"/>
+    </row>
+    <row r="10" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="56" t="s">
         <v>229</v>
       </c>
-      <c r="C8" s="59"/>
-    </row>
-    <row r="9" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="63" t="s">
-        <v>231</v>
-      </c>
-      <c r="B9" s="64"/>
-      <c r="C9" s="65"/>
-    </row>
-    <row r="10" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="58" t="s">
+      <c r="B10" s="65"/>
+      <c r="C10" s="57"/>
+    </row>
+    <row r="11" spans="1:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="52" t="s">
         <v>230</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="59"/>
-    </row>
-    <row r="11" spans="1:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="54" t="s">
+      <c r="B11" s="66"/>
+      <c r="C11" s="53"/>
+    </row>
+    <row r="12" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="70"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+    </row>
+    <row r="13" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="74" t="s">
         <v>232</v>
       </c>
-      <c r="B11" s="67"/>
-      <c r="C11" s="55"/>
-    </row>
-    <row r="12" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="71"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="73"/>
-    </row>
-    <row r="13" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="75" t="s">
-        <v>234</v>
-      </c>
-      <c r="B13" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="C13" s="70"/>
+      <c r="B13" s="75" t="s">
+        <v>233</v>
+      </c>
+      <c r="C13" s="69"/>
     </row>
     <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>216</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B16" s="77" t="s">
-        <v>240</v>
-      </c>
-      <c r="C16" s="53"/>
+        <v>235</v>
+      </c>
+      <c r="B16" s="76" t="s">
+        <v>238</v>
+      </c>
+      <c r="C16" s="51"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="55"/>
+        <v>224</v>
+      </c>
+      <c r="B17" s="52"/>
+      <c r="C17" s="53"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="57"/>
+        <v>223</v>
+      </c>
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
     </row>
     <row r="19" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="B19" s="78" t="s">
-        <v>241</v>
-      </c>
-      <c r="C19" s="59"/>
+        <v>240</v>
+      </c>
+      <c r="B19" s="77" t="s">
+        <v>239</v>
+      </c>
+      <c r="C19" s="57"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="63" t="s">
-        <v>243</v>
-      </c>
-      <c r="B20" s="64"/>
-      <c r="C20" s="65"/>
+      <c r="A20" s="61" t="s">
+        <v>271</v>
+      </c>
+      <c r="B20" s="62"/>
+      <c r="C20" s="63"/>
     </row>
     <row r="21" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="60" t="s">
-        <v>238</v>
-      </c>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
+      <c r="A21" s="58" t="s">
+        <v>236</v>
+      </c>
+      <c r="B21" s="59"/>
+      <c r="C21" s="60"/>
     </row>
     <row r="22" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="63" t="s">
-        <v>239</v>
-      </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="65"/>
+      <c r="A22" s="61" t="s">
+        <v>237</v>
+      </c>
+      <c r="B22" s="62"/>
+      <c r="C22" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -6064,10 +6701,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -6080,103 +6717,295 @@
     <col min="6" max="16384" width="11.5546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>233</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-    </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>217</v>
-      </c>
-      <c r="C2" s="51"/>
+    <row r="1" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="73" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="72"/>
+    </row>
+    <row r="2" spans="1:5" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="74" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="69"/>
       <c r="E2" s="49" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>216</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="36" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="76" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" s="51"/>
+    </row>
+    <row r="6" spans="1:5" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B6" s="52"/>
+      <c r="C6" s="53"/>
+    </row>
+    <row r="7" spans="1:5" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+    </row>
+    <row r="8" spans="1:5" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8" s="77" t="s">
+        <v>255</v>
+      </c>
+      <c r="C8" s="57"/>
+    </row>
+    <row r="9" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="61" t="s">
+        <v>263</v>
+      </c>
+      <c r="B9" s="62"/>
+      <c r="C9" s="63"/>
+    </row>
+    <row r="10" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="56" t="s">
+        <v>229</v>
+      </c>
+      <c r="B10" s="65"/>
+      <c r="C10" s="57"/>
+    </row>
+    <row r="11" spans="1:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="52" t="s">
+        <v>244</v>
+      </c>
+      <c r="B11" s="66"/>
+      <c r="C11" s="53"/>
+    </row>
+    <row r="12" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="70"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+    </row>
+    <row r="13" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="74" t="s">
+        <v>248</v>
+      </c>
+      <c r="B13" s="75" t="s">
+        <v>257</v>
+      </c>
+      <c r="C13" s="69"/>
+    </row>
+    <row r="14" spans="1:5" ht="108" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="36" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B16" s="76" t="s">
+        <v>259</v>
+      </c>
+      <c r="C16" s="51"/>
+    </row>
+    <row r="17" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B17" s="52"/>
+      <c r="C17" s="53"/>
+    </row>
+    <row r="18" spans="1:3" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+    </row>
+    <row r="19" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B19" s="77" t="s">
+        <v>261</v>
+      </c>
+      <c r="C19" s="57"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="61" t="s">
+        <v>262</v>
+      </c>
+      <c r="B20" s="62"/>
+      <c r="C20" s="63"/>
+    </row>
+    <row r="21" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="56" t="s">
+        <v>236</v>
+      </c>
+      <c r="B21" s="65"/>
+      <c r="C21" s="57"/>
+    </row>
+    <row r="22" spans="1:3" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="52" t="s">
+        <v>245</v>
+      </c>
+      <c r="B22" s="66"/>
+      <c r="C22" s="53"/>
+    </row>
+    <row r="23" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="70"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="72"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="B24" s="75" t="s">
+        <v>264</v>
+      </c>
+      <c r="C24" s="69"/>
+    </row>
+    <row r="25" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="C25" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B5" s="52" t="s">
+    </row>
+    <row r="27" spans="1:3" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B27" s="76" t="s">
+        <v>266</v>
+      </c>
+      <c r="C27" s="51"/>
+    </row>
+    <row r="28" spans="1:3" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B28" s="52"/>
+      <c r="C28" s="53"/>
+    </row>
+    <row r="29" spans="1:3" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C5" s="53"/>
-    </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
-    </row>
-    <row r="7" spans="1:5" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="57"/>
-    </row>
-    <row r="8" spans="1:5" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B8" s="58" t="s">
+      <c r="B29" s="54"/>
+      <c r="C29" s="55"/>
+    </row>
+    <row r="30" spans="1:3" ht="108" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B30" s="77" t="s">
+        <v>267</v>
+      </c>
+      <c r="C30" s="57"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="61" t="s">
+        <v>269</v>
+      </c>
+      <c r="B31" s="62"/>
+      <c r="C31" s="63"/>
+    </row>
+    <row r="32" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="56" t="s">
         <v>229</v>
       </c>
-      <c r="C8" s="59"/>
-    </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="63" t="s">
-        <v>231</v>
-      </c>
-      <c r="B9" s="64"/>
-      <c r="C9" s="65"/>
-    </row>
-    <row r="10" spans="1:5" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="60" t="s">
-        <v>230</v>
-      </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="62"/>
-    </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="63" t="s">
-        <v>232</v>
-      </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="65"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="57"/>
+    </row>
+    <row r="33" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="54" t="s">
+        <v>246</v>
+      </c>
+      <c r="B33" s="64"/>
+      <c r="C33" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="21">
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B27:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A31:C31"/>
     <mergeCell ref="A11:C11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B16:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B5:C7"/>

</xml_diff>

<commit_message>
✨ Adding screenshots of step-by-step defect replication process
</commit_message>
<xml_diff>
--- a/PlanDePruebasRiesgosCasosDePrueba.xlsx
+++ b/PlanDePruebasRiesgosCasosDePrueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sofka\Training\Duras\Repos\C1-2023-QA-Calidad-T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4214BD39-8C5A-416C-8310-6B5B21C905FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88522828-6CBF-43A2-AA7D-66838150E1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AF02FBB8-0A87-4B34-9297-94FCF679C14E}"/>
   </bookViews>
@@ -1582,40 +1582,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Descripción:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Para lograr reproducir este bug, es necesario seguir los pasos siguientes:
-1. Ingresar a la aplicación Postman.
-2. Crear una nueva HTTP Request de tipo POST.
-3. Ingresar la URL https://reqres.in/api/register.
-4. Ingresar un cuerpo con el siguiente formato:
-  {
-    "email": "eve.holt@reqres.in",
-    "password": "pass"
-  }
-5. Enviar la petición.
-6. Visualizar el código de respuesta OK y token de registro.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Resultados Obtenidos:</t>
     </r>
     <r>
@@ -2454,6 +2420,40 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> base de datos y área de seguridad.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descripción:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Para lograr reproducir este bug, es necesario seguir los pasos siguientes:
+1. Ingresar a la aplicación Postman.
+2. Crear una nueva HTTP Request de tipo POST.
+3. Ingresar la URL https://reqres.in/api/register.
+4. Ingresar un cuerpo con el siguiente formato:
+  {
+                                                                     "email": "eve.holt@reqres.in",
+                                                "password": "pass"
+  }
+5. Enviar la petición.
+6. Visualizar el código de respuesta OK y token de registro.</t>
     </r>
   </si>
 </sst>
@@ -6486,7 +6486,7 @@
     <col min="1" max="1" width="36" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="5"/>
+    <col min="4" max="4" width="12.109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="61.6640625" style="5" customWidth="1"/>
     <col min="6" max="16384" width="11.5546875" style="5"/>
   </cols>
@@ -6507,7 +6507,7 @@
       </c>
       <c r="C2" s="69"/>
       <c r="E2" s="49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.3">
@@ -6518,7 +6518,7 @@
         <v>218</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -6566,7 +6566,7 @@
     </row>
     <row r="9" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B9" s="62"/>
       <c r="C9" s="63"/>
@@ -6607,7 +6607,7 @@
         <v>234</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -6621,23 +6621,23 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>235</v>
       </c>
       <c r="B16" s="76" t="s">
-        <v>238</v>
+        <v>271</v>
       </c>
       <c r="C16" s="51"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>224</v>
       </c>
       <c r="B17" s="52"/>
       <c r="C17" s="53"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>223</v>
       </c>
@@ -6646,16 +6646,16 @@
     </row>
     <row r="19" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B19" s="77" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C19" s="57"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="61" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B20" s="62"/>
       <c r="C20" s="63"/>
@@ -6726,10 +6726,10 @@
     </row>
     <row r="2" spans="1:5" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="74" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="75" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C2" s="69"/>
       <c r="E2" s="49" t="s">
@@ -6744,7 +6744,7 @@
         <v>218</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="36" x14ac:dyDescent="0.3">
@@ -6752,7 +6752,7 @@
         <v>219</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>221</v>
@@ -6763,13 +6763,13 @@
         <v>225</v>
       </c>
       <c r="B5" s="76" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C5" s="51"/>
     </row>
     <row r="6" spans="1:5" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B6" s="52"/>
       <c r="C6" s="53"/>
@@ -6783,16 +6783,16 @@
     </row>
     <row r="8" spans="1:5" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B8" s="77" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="57"/>
     </row>
     <row r="9" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="61" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B9" s="62"/>
       <c r="C9" s="63"/>
@@ -6806,7 +6806,7 @@
     </row>
     <row r="11" spans="1:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="52" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B11" s="66"/>
       <c r="C11" s="53"/>
@@ -6818,10 +6818,10 @@
     </row>
     <row r="13" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="74" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B13" s="75" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C13" s="69"/>
     </row>
@@ -6833,7 +6833,7 @@
         <v>234</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="36" x14ac:dyDescent="0.3">
@@ -6841,7 +6841,7 @@
         <v>219</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>221</v>
@@ -6852,7 +6852,7 @@
         <v>235</v>
       </c>
       <c r="B16" s="76" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C16" s="51"/>
     </row>
@@ -6872,16 +6872,16 @@
     </row>
     <row r="19" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B19" s="77" t="s">
         <v>260</v>
-      </c>
-      <c r="B19" s="77" t="s">
-        <v>261</v>
       </c>
       <c r="C19" s="57"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="61" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B20" s="62"/>
       <c r="C20" s="63"/>
@@ -6895,7 +6895,7 @@
     </row>
     <row r="22" spans="1:3" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="52" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B22" s="66"/>
       <c r="C22" s="53"/>
@@ -6907,10 +6907,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="74" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B24" s="75" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C24" s="69"/>
     </row>
@@ -6922,7 +6922,7 @@
         <v>218</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="36" x14ac:dyDescent="0.3">
@@ -6930,7 +6930,7 @@
         <v>219</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>221</v>
@@ -6941,7 +6941,7 @@
         <v>235</v>
       </c>
       <c r="B27" s="76" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C27" s="51"/>
     </row>
@@ -6961,16 +6961,16 @@
     </row>
     <row r="30" spans="1:3" ht="108" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B30" s="77" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C30" s="57"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="61" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B31" s="62"/>
       <c r="C31" s="63"/>
@@ -6984,7 +6984,7 @@
     </row>
     <row r="33" spans="1:3" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="54" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B33" s="64"/>
       <c r="C33" s="55"/>

</xml_diff>